<commit_message>
Revert "Add Israel and South Korea To All Cause Analysis"
This reverts commit 306f4cb4c53c92e7ec3d4479405d34e46d297d62.
</commit_message>
<xml_diff>
--- a/out/tab_ex_diff.xlsx
+++ b/out/tab_ex_diff.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1148" uniqueCount="1026">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1112" uniqueCount="990">
   <si>
     <t xml:space="preserve">Region ISO</t>
   </si>
@@ -1040,109 +1040,58 @@
     <t xml:space="preserve">+0.23 (+0.19,+0.27)</t>
   </si>
   <si>
-    <t xml:space="preserve">IL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Israel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.92 (83.76,84.08)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.78 (79.62,79.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.15 (84.01,84.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.46 (80.31,80.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.54 (84.39,84.69)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.36 (80.22,80.53)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.75 (84.61,84.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.73 (80.58,80.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.59 (84.44,84.74)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.79 (80.61,80.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.49 (84.35,84.61)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.28 (80.14,80.43)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.10 (-0.30,+0.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.50 (-0.72,-0.26)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.25 (+0.20,+0.30)</t>
-  </si>
-  <si>
     <t xml:space="preserve">IS</t>
   </si>
   <si>
     <t xml:space="preserve">Iceland</t>
   </si>
   <si>
-    <t xml:space="preserve">83.52 (82.86,84.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.88 (80.24,81.64)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.79 (83.16,84.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.29 (79.70,81.01)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.02 (83.38,84.72)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.90 (80.29,81.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.25 (83.57,84.95)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.03 (80.33,81.74)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.42 (83.78,85.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.28 (80.68,82.01)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.34 (83.76,85.03)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.08 (80.35,81.85)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.07 (-0.99,+0.81)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.20 (-1.16,+0.73)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.22 (-0.01,+0.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.10 (-0.13,+0.35)</t>
+    <t xml:space="preserve">83.52 (82.89,84.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.88 (80.22,81.65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.79 (83.22,84.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.29 (79.66,80.90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.02 (83.39,84.69)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.90 (80.16,81.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.25 (83.65,84.90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.03 (80.36,81.75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.42 (83.81,85.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.28 (80.54,81.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.34 (83.71,85.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.08 (80.46,81.80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.07 (-0.95,+0.90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.20 (-1.18,+0.84)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.22 (+0.01,+0.44)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.10 (-0.17,+0.34)</t>
   </si>
   <si>
     <t xml:space="preserve">IT</t>
@@ -1154,13 +1103,13 @@
     <t xml:space="preserve">84.37 (84.33,84.42)</t>
   </si>
   <si>
-    <t xml:space="preserve">79.89 (79.85,79.94)</t>
+    <t xml:space="preserve">79.89 (79.85,79.93)</t>
   </si>
   <si>
     <t xml:space="preserve">85.14 (85.09,85.19)</t>
   </si>
   <si>
-    <t xml:space="preserve">80.59 (80.55,80.64)</t>
+    <t xml:space="preserve">80.59 (80.54,80.63)</t>
   </si>
   <si>
     <t xml:space="preserve">84.81 (84.77,84.85)</t>
@@ -1175,19 +1124,22 @@
     <t xml:space="preserve">80.85 (80.80,80.90)</t>
   </si>
   <si>
+    <t xml:space="preserve">85.36 (85.31,85.40)</t>
+  </si>
+  <si>
     <t xml:space="preserve">81.08 (81.03,81.12)</t>
   </si>
   <si>
-    <t xml:space="preserve">84.35 (84.31,84.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.83 (79.79,79.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.01 (-1.07,-0.96)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.25 (-1.31,-1.19)</t>
+    <t xml:space="preserve">84.35 (84.30,84.39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.83 (79.78,79.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.01 (-1.07,-0.95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.25 (-1.31,-1.18)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.25 (+0.23,+0.26)</t>
@@ -1196,106 +1148,52 @@
     <t xml:space="preserve">+0.30 (+0.28,+0.31)</t>
   </si>
   <si>
-    <t xml:space="preserve">KR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">South Korea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85.52 (85.46,85.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.82 (78.75,78.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">85.88 (85.82,85.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.28 (79.22,79.34)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86.14 (86.08,86.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.63 (79.56,79.70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86.06 (86.00,86.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.62 (79.56,79.69)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86.75 (86.68,86.82)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.15 (80.09,80.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">86.86 (86.80,86.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.38 (80.33,80.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.11 (+0.01,+0.20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.23 (+0.14,+0.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.31 (+0.28,+0.33)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.33 (+0.31,+0.36)</t>
-  </si>
-  <si>
     <t xml:space="preserve">LT</t>
   </si>
   <si>
     <t xml:space="preserve">Lithuania</t>
   </si>
   <si>
-    <t xml:space="preserve">79.61 (79.41,79.81)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69.11 (68.86,69.34)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.20 (79.97,80.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69.57 (69.34,69.80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.62 (80.40,80.85)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70.82 (70.61,71.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.91 (80.68,81.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70.96 (70.69,71.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.42 (81.19,81.64)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71.38 (71.15,71.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.16 (79.95,80.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69.69 (69.49,69.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.26 (-1.59,-0.96)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.69 (-2.01,-1.36)</t>
+    <t xml:space="preserve">79.61 (79.39,79.82)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.11 (68.92,69.33)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.20 (80.00,80.41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.57 (69.33,69.78)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.62 (80.40,80.82)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70.82 (70.59,71.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.91 (80.66,81.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70.96 (70.75,71.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.42 (81.20,81.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71.38 (71.15,71.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.16 (79.95,80.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.69 (69.48,69.94)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.26 (-1.54,-0.97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.69 (-2.00,-1.36)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.45 (+0.38,+0.53)</t>
@@ -1310,28 +1208,28 @@
     <t xml:space="preserve">Netherlands</t>
   </si>
   <si>
-    <t xml:space="preserve">83.01 (82.94,83.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.68 (79.60,79.76)</t>
+    <t xml:space="preserve">83.01 (82.94,83.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.68 (79.61,79.76)</t>
   </si>
   <si>
     <t xml:space="preserve">83.08 (82.99,83.16)</t>
   </si>
   <si>
-    <t xml:space="preserve">79.94 (79.84,80.03)</t>
+    <t xml:space="preserve">79.94 (79.86,80.01)</t>
   </si>
   <si>
     <t xml:space="preserve">83.25 (83.17,83.34)</t>
   </si>
   <si>
-    <t xml:space="preserve">80.15 (80.06,80.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.26 (83.18,83.36)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.26 (80.18,80.35)</t>
+    <t xml:space="preserve">80.15 (80.06,80.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.26 (83.18,83.35)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.26 (80.17,80.34)</t>
   </si>
   <si>
     <t xml:space="preserve">83.52 (83.43,83.60)</t>
@@ -1340,13 +1238,13 @@
     <t xml:space="preserve">80.58 (80.50,80.67)</t>
   </si>
   <si>
-    <t xml:space="preserve">82.95 (82.87,83.04)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.78 (79.69,79.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.57 (-0.68,-0.44)</t>
+    <t xml:space="preserve">82.95 (82.88,83.03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.78 (79.70,79.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.57 (-0.68,-0.46)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.80 (-0.92,-0.68)</t>
@@ -1355,58 +1253,55 @@
     <t xml:space="preserve">+0.13 (+0.10,+0.15)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.23 (+0.20,+0.26)</t>
-  </si>
-  <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
     <t xml:space="preserve">Norway</t>
   </si>
   <si>
-    <t xml:space="preserve">83.88 (83.73,84.04)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.25 (80.11,80.42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.98 (83.82,84.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.64 (80.49,80.79)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.09 (83.94,84.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.90 (80.73,81.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.26 (84.12,84.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.00 (80.86,81.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.44 (84.29,84.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.17 (81.02,81.34)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.62 (84.47,84.78)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.36 (81.21,81.52)</t>
+    <t xml:space="preserve">83.88 (83.71,84.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.25 (80.09,80.40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.98 (83.83,84.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.64 (80.47,80.81)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.09 (83.95,84.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.90 (80.71,81.06)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.26 (84.10,84.42)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.00 (80.85,81.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.44 (84.26,84.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.17 (81.00,81.34)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.62 (84.47,84.76)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.36 (81.21,81.51)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.18 (-0.04,+0.40)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.18 (-0.03,+0.41)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.14 (+0.09,+0.19)</t>
+    <t xml:space="preserve">+0.18 (-0.04,+0.42)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.14 (+0.08,+0.19)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.23 (+0.17,+0.29)</t>
@@ -1421,7 +1316,7 @@
     <t xml:space="preserve">81.35 (81.29,81.41)</t>
   </si>
   <si>
-    <t xml:space="preserve">73.40 (73.33,73.46)</t>
+    <t xml:space="preserve">73.40 (73.34,73.46)</t>
   </si>
   <si>
     <t xml:space="preserve">81.89 (81.83,81.96)</t>
@@ -1430,31 +1325,31 @@
     <t xml:space="preserve">73.85 (73.78,73.91)</t>
   </si>
   <si>
-    <t xml:space="preserve">81.64 (81.58,81.70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.83 (73.76,73.90)</t>
+    <t xml:space="preserve">81.64 (81.59,81.70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.83 (73.76,73.89)</t>
   </si>
   <si>
     <t xml:space="preserve">81.66 (81.60,81.72)</t>
   </si>
   <si>
-    <t xml:space="preserve">73.81 (73.74,73.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.96 (81.90,82.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.20 (74.13,74.27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.89 (80.83,80.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72.70 (72.64,72.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.07 (-1.15,-0.99)</t>
+    <t xml:space="preserve">73.81 (73.74,73.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.96 (81.91,82.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.20 (74.14,74.26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.89 (80.84,80.94)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72.70 (72.65,72.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.07 (-1.15,-1.00)</t>
   </si>
   <si>
     <t xml:space="preserve">-1.50 (-1.58,-1.41)</t>
@@ -1472,52 +1367,52 @@
     <t xml:space="preserve">Portugal</t>
   </si>
   <si>
-    <t xml:space="preserve">83.87 (83.76,83.96)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.03 (77.91,78.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.02 (83.91,84.11)</t>
+    <t xml:space="preserve">83.87 (83.78,83.97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.03 (77.92,78.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.02 (83.91,84.12)</t>
   </si>
   <si>
     <t xml:space="preserve">78.09 (77.97,78.21)</t>
   </si>
   <si>
-    <t xml:space="preserve">84.29 (84.19,84.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.41 (78.29,78.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.20 (84.10,84.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.33 (78.21,78.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.48 (84.37,84.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.69 (78.57,78.82)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.79 (83.70,83.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.86 (77.74,77.98)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.69 (-0.83,-0.54)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83 (-0.99,-0.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.15 (+0.12,+0.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.17 (+0.12,+0.20)</t>
+    <t xml:space="preserve">84.29 (84.18,84.40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.41 (78.29,78.53)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.20 (84.09,84.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.33 (78.22,78.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.48 (84.37,84.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.69 (78.58,78.81)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.79 (83.67,83.90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.86 (77.75,77.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.69 (-0.84,-0.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.83 (-1.02,-0.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.15 (+0.11,+0.19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.17 (+0.13,+0.21)</t>
   </si>
   <si>
     <t xml:space="preserve">SE</t>
@@ -1532,46 +1427,46 @@
     <t xml:space="preserve">80.14 (80.04,80.25)</t>
   </si>
   <si>
-    <t xml:space="preserve">83.88 (83.77,83.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.47 (80.35,80.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.88 (83.78,83.97)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.59 (80.49,80.69)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.00 (83.89,84.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.66 (80.56,80.78)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.49 (84.38,84.61)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.18 (81.06,81.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.90 (83.80,83.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.31 (80.20,80.41)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.59 (-0.74,-0.46)</t>
+    <t xml:space="preserve">83.88 (83.77,83.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.47 (80.35,80.57)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.88 (83.78,83.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.59 (80.48,80.69)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.00 (83.90,84.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.66 (80.56,80.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.49 (84.38,84.60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.18 (81.07,81.29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.90 (83.78,83.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.31 (80.21,80.41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.59 (-0.76,-0.46)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.87 (-1.02,-0.72)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.18 (+0.15,+0.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.26 (+0.22,+0.29)</t>
+    <t xml:space="preserve">+0.18 (+0.14,+0.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.26 (+0.22,+0.30)</t>
   </si>
   <si>
     <t xml:space="preserve">SI</t>
@@ -1580,46 +1475,46 @@
     <t xml:space="preserve">Slovenia</t>
   </si>
   <si>
-    <t xml:space="preserve">83.60 (83.36,83.84)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.68 (77.42,77.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.04 (83.82,84.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.15 (77.91,78.40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.85 (83.62,84.08)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.25 (78.00,78.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.13 (83.87,84.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.47 (78.23,78.73)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.25 (84.03,84.47)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.63 (78.38,78.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.19 (82.98,83.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.68 (77.45,77.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.06 (-1.35,-0.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.94 (-1.26,-0.60)</t>
+    <t xml:space="preserve">83.60 (83.36,83.82)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.68 (77.47,77.95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.04 (83.83,84.26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.15 (77.91,78.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.85 (83.63,84.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.25 (78.00,78.49)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.13 (83.88,84.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.47 (78.26,78.74)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.25 (84.02,84.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.63 (78.37,78.91)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.19 (82.99,83.39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.68 (77.47,77.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.06 (-1.35,-0.71)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.94 (-1.29,-0.57)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.16 (+0.08,+0.24)</t>
@@ -1637,49 +1532,49 @@
     <t xml:space="preserve">80.01 (79.86,80.16)</t>
   </si>
   <si>
-    <t xml:space="preserve">73.00 (72.83,73.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.53 (80.37,80.68)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.74 (73.58,73.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.52 (80.37,80.66)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.73 (73.59,73.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.56 (80.42,80.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.82 (73.65,73.97)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.92 (80.78,81.06)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.20 (74.04,74.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.14 (79.99,80.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.38 (73.23,73.54)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.79 (-0.98,-0.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83 (-1.04,-0.57)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.23 (+0.17,+0.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.30 (+0.24,+0.37)</t>
+    <t xml:space="preserve">73.00 (72.84,73.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.53 (80.39,80.69)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.74 (73.57,73.90)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.52 (80.37,80.65)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.73 (73.56,73.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.56 (80.40,80.71)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.82 (73.66,73.97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.92 (80.77,81.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.20 (74.02,74.37)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.14 (80.00,80.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.38 (73.21,73.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.79 (-0.99,-0.58)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.83 (-1.07,-0.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.23 (+0.18,+0.28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.30 (+0.24,+0.36)</t>
   </si>
   <si>
     <t xml:space="preserve">US</t>
@@ -1691,10 +1586,10 @@
     <t xml:space="preserve">81.17 (81.15,81.20)</t>
   </si>
   <si>
-    <t xml:space="preserve">76.47 (76.45,76.50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.30 (81.27,81.32)</t>
+    <t xml:space="preserve">76.47 (76.44,76.50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.30 (81.28,81.32)</t>
   </si>
   <si>
     <t xml:space="preserve">76.45 (76.43,76.48)</t>
@@ -1715,7 +1610,7 @@
     <t xml:space="preserve">81.65 (81.62,81.67)</t>
   </si>
   <si>
-    <t xml:space="preserve">76.74 (76.71,76.77)</t>
+    <t xml:space="preserve">76.74 (76.72,76.76)</t>
   </si>
   <si>
     <t xml:space="preserve">80.00 (79.98,80.02)</t>
@@ -1727,7 +1622,7 @@
     <t xml:space="preserve">-1.65 (-1.68,-1.62)</t>
   </si>
   <si>
-    <t xml:space="preserve">-2.23 (-2.26,-2.19)</t>
+    <t xml:space="preserve">-2.23 (-2.26,-2.20)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.12 (+0.11,+0.13)</t>
@@ -2451,9 +2346,6 @@
   </si>
   <si>
     <t xml:space="preserve">-0.87 (-1.03,-0.72)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.15 (+0.11,+0.19)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.21 (+0.17,+0.25)</t>
@@ -3216,20 +3108,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:R31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O27" activeCellId="0" sqref="O27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="19.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4396,682 +4288,570 @@
         <v>354</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>160</v>
+        <v>355</v>
       </c>
       <c r="R21" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="R22" s="0" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>221</v>
+        <v>385</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="R23" s="0" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="R24" s="0" t="s">
-        <v>408</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
         <v>535</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>536</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>537</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>538</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>539</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>540</v>
-      </c>
-      <c r="G32" s="0" t="s">
-        <v>541</v>
-      </c>
-      <c r="H32" s="0" t="s">
-        <v>542</v>
-      </c>
-      <c r="I32" s="0" t="s">
-        <v>543</v>
-      </c>
-      <c r="J32" s="0" t="s">
-        <v>544</v>
-      </c>
-      <c r="K32" s="0" t="s">
-        <v>545</v>
-      </c>
-      <c r="L32" s="0" t="s">
-        <v>546</v>
-      </c>
-      <c r="M32" s="0" t="s">
-        <v>547</v>
-      </c>
-      <c r="N32" s="0" t="s">
-        <v>548</v>
-      </c>
-      <c r="O32" s="0" t="s">
-        <v>549</v>
-      </c>
-      <c r="P32" s="0" t="s">
-        <v>550</v>
-      </c>
-      <c r="Q32" s="0" t="s">
-        <v>551</v>
-      </c>
-      <c r="R32" s="0" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>553</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>554</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>555</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>556</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>557</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>558</v>
-      </c>
-      <c r="G33" s="0" t="s">
-        <v>559</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>560</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>561</v>
-      </c>
-      <c r="J33" s="0" t="s">
-        <v>562</v>
-      </c>
-      <c r="K33" s="0" t="s">
-        <v>563</v>
-      </c>
-      <c r="L33" s="0" t="s">
-        <v>564</v>
-      </c>
-      <c r="M33" s="0" t="s">
-        <v>565</v>
-      </c>
-      <c r="N33" s="0" t="s">
-        <v>566</v>
-      </c>
-      <c r="O33" s="0" t="s">
-        <v>567</v>
-      </c>
-      <c r="P33" s="0" t="s">
-        <v>568</v>
-      </c>
-      <c r="Q33" s="0" t="s">
-        <v>569</v>
-      </c>
-      <c r="R33" s="0" t="s">
-        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -5108,12 +4888,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="19.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="3" style="0" width="19.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="15" style="0" width="18.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="0" width="18.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="10.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5124,49 +4904,49 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>571</v>
+        <v>536</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>572</v>
+        <v>537</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>573</v>
+        <v>538</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>574</v>
+        <v>539</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>575</v>
+        <v>540</v>
       </c>
       <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>576</v>
+        <v>541</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>577</v>
+        <v>542</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>578</v>
+        <v>543</v>
       </c>
       <c r="R1" s="3" t="s">
         <v>17</v>
@@ -5230,52 +5010,52 @@
         <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>579</v>
+        <v>544</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>580</v>
+        <v>545</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>581</v>
+        <v>546</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>582</v>
+        <v>547</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>583</v>
+        <v>548</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>584</v>
+        <v>549</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>585</v>
+        <v>550</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>586</v>
+        <v>551</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>587</v>
+        <v>552</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>588</v>
+        <v>553</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>589</v>
+        <v>554</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>590</v>
+        <v>555</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>591</v>
+        <v>556</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>592</v>
+        <v>557</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>593</v>
+        <v>558</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>594</v>
+        <v>559</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5286,52 +5066,52 @@
         <v>39</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>595</v>
+        <v>560</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>596</v>
+        <v>561</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>597</v>
+        <v>562</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>598</v>
+        <v>563</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>599</v>
+        <v>564</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>600</v>
+        <v>565</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>601</v>
+        <v>566</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>602</v>
+        <v>567</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>603</v>
+        <v>568</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>604</v>
+        <v>569</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>605</v>
+        <v>570</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>606</v>
+        <v>571</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>607</v>
+        <v>572</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>608</v>
+        <v>573</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>609</v>
+        <v>574</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>610</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5342,52 +5122,52 @@
         <v>57</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>611</v>
+        <v>576</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>612</v>
+        <v>577</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>613</v>
+        <v>578</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>614</v>
+        <v>579</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>615</v>
+        <v>580</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>616</v>
+        <v>581</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>617</v>
+        <v>582</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>614</v>
+        <v>579</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>618</v>
+        <v>583</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>619</v>
+        <v>584</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>620</v>
+        <v>585</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>621</v>
+        <v>586</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>622</v>
+        <v>587</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>623</v>
+        <v>588</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>625</v>
+        <v>590</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5398,52 +5178,52 @@
         <v>75</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>626</v>
+        <v>591</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>627</v>
+        <v>592</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>628</v>
+        <v>593</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>629</v>
+        <v>594</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>630</v>
+        <v>595</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>631</v>
+        <v>596</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>632</v>
+        <v>597</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>633</v>
+        <v>598</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>634</v>
+        <v>599</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>635</v>
+        <v>600</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>636</v>
+        <v>601</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>637</v>
+        <v>602</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>638</v>
+        <v>603</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>639</v>
+        <v>604</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>640</v>
+        <v>605</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>641</v>
+        <v>606</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5460,46 +5240,46 @@
         <v>94</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>642</v>
+        <v>607</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>643</v>
+        <v>608</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>644</v>
+        <v>609</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>645</v>
+        <v>610</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>646</v>
+        <v>611</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>647</v>
+        <v>612</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>648</v>
+        <v>613</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>649</v>
+        <v>614</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>650</v>
+        <v>615</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>611</v>
+        <v>576</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>651</v>
+        <v>616</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>652</v>
+        <v>617</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>653</v>
+        <v>618</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>654</v>
+        <v>619</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5510,52 +5290,52 @@
         <v>110</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>655</v>
+        <v>620</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>656</v>
+        <v>621</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>657</v>
+        <v>622</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>658</v>
+        <v>623</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>659</v>
+        <v>624</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>660</v>
+        <v>625</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>661</v>
+        <v>626</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>662</v>
+        <v>627</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>663</v>
+        <v>628</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>664</v>
+        <v>629</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>665</v>
+        <v>630</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>666</v>
+        <v>631</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>667</v>
+        <v>632</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>668</v>
+        <v>633</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>669</v>
+        <v>634</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>670</v>
+        <v>635</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5572,46 +5352,46 @@
         <v>94</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>671</v>
+        <v>636</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>672</v>
+        <v>637</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>673</v>
+        <v>638</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>674</v>
+        <v>639</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>675</v>
+        <v>640</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>676</v>
+        <v>641</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>677</v>
+        <v>642</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>678</v>
+        <v>643</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>679</v>
+        <v>644</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>680</v>
+        <v>645</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>681</v>
+        <v>646</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>682</v>
+        <v>647</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>683</v>
+        <v>648</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>684</v>
+        <v>649</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5622,52 +5402,52 @@
         <v>144</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>685</v>
+        <v>650</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>686</v>
+        <v>651</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>687</v>
+        <v>652</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>688</v>
+        <v>653</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>689</v>
+        <v>654</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>690</v>
+        <v>655</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>691</v>
+        <v>656</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>692</v>
+        <v>657</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>693</v>
+        <v>658</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>694</v>
+        <v>659</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>695</v>
+        <v>660</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>696</v>
+        <v>661</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>697</v>
+        <v>662</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>698</v>
+        <v>663</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>699</v>
+        <v>664</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>700</v>
+        <v>665</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5678,49 +5458,49 @@
         <v>162</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>701</v>
+        <v>666</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>702</v>
+        <v>667</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>703</v>
+        <v>668</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>704</v>
+        <v>669</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>705</v>
+        <v>670</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>706</v>
+        <v>671</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>707</v>
+        <v>672</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>708</v>
+        <v>673</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>709</v>
+        <v>674</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>710</v>
+        <v>675</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>711</v>
+        <v>676</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>712</v>
+        <v>677</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>713</v>
+        <v>678</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>714</v>
+        <v>679</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>715</v>
+        <v>680</v>
       </c>
       <c r="R11" s="0" t="s">
         <v>267</v>
@@ -5734,52 +5514,52 @@
         <v>180</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>716</v>
+        <v>681</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>717</v>
+        <v>682</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>718</v>
+        <v>683</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>719</v>
+        <v>684</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>720</v>
+        <v>685</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>721</v>
+        <v>686</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>722</v>
+        <v>687</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>723</v>
+        <v>688</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>724</v>
+        <v>689</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>725</v>
+        <v>690</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>726</v>
+        <v>691</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>727</v>
+        <v>692</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>728</v>
+        <v>693</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>729</v>
+        <v>694</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>730</v>
+        <v>695</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>731</v>
+        <v>696</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5790,52 +5570,52 @@
         <v>198</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>732</v>
+        <v>697</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>733</v>
+        <v>698</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>734</v>
+        <v>699</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>735</v>
+        <v>700</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>736</v>
+        <v>701</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>737</v>
+        <v>702</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>738</v>
+        <v>703</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>739</v>
+        <v>704</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>740</v>
+        <v>705</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>741</v>
+        <v>706</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>742</v>
+        <v>707</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>743</v>
+        <v>708</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>744</v>
+        <v>709</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>745</v>
+        <v>710</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>746</v>
+        <v>711</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>747</v>
+        <v>712</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5846,52 +5626,52 @@
         <v>216</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>748</v>
+        <v>713</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>749</v>
+        <v>714</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>750</v>
+        <v>715</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>751</v>
+        <v>716</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>752</v>
+        <v>717</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>753</v>
+        <v>718</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>754</v>
+        <v>719</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>755</v>
+        <v>720</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>756</v>
+        <v>721</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>757</v>
+        <v>722</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>758</v>
+        <v>723</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>759</v>
+        <v>724</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>760</v>
+        <v>725</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>761</v>
+        <v>726</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>762</v>
+        <v>727</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>763</v>
+        <v>728</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5902,52 +5682,52 @@
         <v>234</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>764</v>
+        <v>729</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>765</v>
+        <v>730</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>766</v>
+        <v>731</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>767</v>
+        <v>732</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>768</v>
+        <v>733</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>769</v>
+        <v>734</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>770</v>
+        <v>735</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>771</v>
+        <v>736</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>772</v>
+        <v>737</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>773</v>
+        <v>738</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>774</v>
+        <v>739</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>775</v>
+        <v>740</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>776</v>
+        <v>741</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>777</v>
+        <v>742</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>778</v>
+        <v>743</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>779</v>
+        <v>744</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5958,52 +5738,52 @@
         <v>252</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>780</v>
+        <v>745</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>781</v>
+        <v>746</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>782</v>
+        <v>747</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>783</v>
+        <v>748</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>784</v>
+        <v>749</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>785</v>
+        <v>750</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>786</v>
+        <v>751</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>787</v>
+        <v>752</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>788</v>
+        <v>753</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>789</v>
+        <v>754</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>790</v>
+        <v>755</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>791</v>
+        <v>756</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>792</v>
+        <v>757</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>793</v>
+        <v>758</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>794</v>
+        <v>759</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>795</v>
+        <v>760</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6014,52 +5794,52 @@
         <v>270</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>796</v>
+        <v>761</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>797</v>
+        <v>762</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>798</v>
+        <v>763</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>799</v>
+        <v>764</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>800</v>
+        <v>765</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>801</v>
+        <v>766</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>802</v>
+        <v>767</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>803</v>
+        <v>768</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>804</v>
+        <v>769</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>805</v>
+        <v>770</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>806</v>
+        <v>771</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>807</v>
+        <v>772</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>808</v>
+        <v>773</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>809</v>
+        <v>774</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>810</v>
+        <v>462</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>811</v>
+        <v>775</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6076,46 +5856,46 @@
         <v>94</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>812</v>
+        <v>776</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>813</v>
+        <v>777</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>814</v>
+        <v>778</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>815</v>
+        <v>779</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>816</v>
+        <v>780</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>817</v>
+        <v>781</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>818</v>
+        <v>782</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>819</v>
+        <v>783</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>820</v>
+        <v>784</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>821</v>
+        <v>785</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>822</v>
+        <v>786</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>823</v>
+        <v>787</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>824</v>
+        <v>788</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>825</v>
+        <v>789</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6126,52 +5906,52 @@
         <v>304</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>826</v>
+        <v>790</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>827</v>
+        <v>791</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>828</v>
+        <v>792</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>829</v>
+        <v>793</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>830</v>
+        <v>794</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>831</v>
+        <v>795</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>832</v>
+        <v>796</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>833</v>
+        <v>797</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>834</v>
+        <v>798</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>835</v>
+        <v>799</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>836</v>
+        <v>800</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>837</v>
+        <v>801</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>838</v>
+        <v>802</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>839</v>
+        <v>803</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>811</v>
+        <v>775</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>840</v>
+        <v>804</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6182,668 +5962,668 @@
         <v>322</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>615</v>
+        <v>580</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>841</v>
+        <v>805</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>842</v>
+        <v>806</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>843</v>
+        <v>807</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>844</v>
+        <v>808</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>845</v>
+        <v>809</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>846</v>
+        <v>810</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>847</v>
+        <v>811</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>848</v>
+        <v>812</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>849</v>
+        <v>813</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>850</v>
+        <v>814</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>851</v>
+        <v>815</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>852</v>
+        <v>816</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>853</v>
+        <v>817</v>
       </c>
       <c r="Q20" s="0" t="s">
         <v>142</v>
       </c>
       <c r="R20" s="0" t="s">
-        <v>624</v>
+        <v>589</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>854</v>
+        <v>818</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>855</v>
+        <v>819</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>856</v>
+        <v>820</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>857</v>
+        <v>821</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>858</v>
+        <v>822</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>859</v>
+        <v>823</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>860</v>
+        <v>824</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>861</v>
+        <v>825</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>862</v>
+        <v>826</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>863</v>
+        <v>827</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>864</v>
+        <v>828</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>865</v>
+        <v>829</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>866</v>
+        <v>830</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>867</v>
+        <v>831</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>868</v>
+        <v>832</v>
       </c>
       <c r="R21" s="0" t="s">
-        <v>869</v>
+        <v>833</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>374</v>
+        <v>357</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>375</v>
+        <v>358</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>870</v>
+        <v>834</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>871</v>
+        <v>835</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>872</v>
+        <v>836</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>873</v>
+        <v>837</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>874</v>
+        <v>838</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>875</v>
+        <v>839</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>876</v>
+        <v>840</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>877</v>
+        <v>841</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>878</v>
+        <v>842</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>879</v>
+        <v>843</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>880</v>
+        <v>844</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>881</v>
+        <v>845</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>882</v>
+        <v>846</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>883</v>
+        <v>847</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>884</v>
+        <v>848</v>
       </c>
       <c r="R22" s="0" t="s">
-        <v>885</v>
+        <v>849</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>409</v>
+        <v>375</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>410</v>
+        <v>376</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>886</v>
+        <v>850</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>887</v>
+        <v>851</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>888</v>
+        <v>852</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>889</v>
+        <v>853</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>890</v>
+        <v>854</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>891</v>
+        <v>855</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>892</v>
+        <v>856</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>893</v>
+        <v>857</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>894</v>
+        <v>858</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>895</v>
+        <v>859</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>896</v>
+        <v>860</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>897</v>
+        <v>861</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>898</v>
+        <v>862</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>899</v>
+        <v>863</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>900</v>
+        <v>864</v>
       </c>
       <c r="R23" s="0" t="s">
-        <v>901</v>
+        <v>865</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>427</v>
+        <v>393</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>428</v>
+        <v>394</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>902</v>
+        <v>866</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>903</v>
+        <v>867</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>904</v>
+        <v>868</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>905</v>
+        <v>869</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>906</v>
+        <v>870</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>907</v>
+        <v>871</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>908</v>
+        <v>872</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>909</v>
+        <v>873</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>910</v>
+        <v>874</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>911</v>
+        <v>875</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>912</v>
+        <v>876</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>913</v>
+        <v>877</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>914</v>
+        <v>878</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>915</v>
+        <v>879</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>916</v>
+        <v>880</v>
       </c>
       <c r="R24" s="0" t="s">
-        <v>917</v>
+        <v>881</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>445</v>
+        <v>410</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>446</v>
+        <v>411</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>918</v>
+        <v>882</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>919</v>
+        <v>883</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>920</v>
+        <v>884</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>921</v>
+        <v>885</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>922</v>
+        <v>886</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>923</v>
+        <v>887</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>924</v>
+        <v>888</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>925</v>
+        <v>889</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>926</v>
+        <v>890</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>927</v>
+        <v>891</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>928</v>
+        <v>892</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>929</v>
+        <v>893</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>930</v>
+        <v>894</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>931</v>
+        <v>895</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>699</v>
+        <v>664</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>840</v>
+        <v>804</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>463</v>
+        <v>428</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>464</v>
+        <v>429</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>932</v>
+        <v>896</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>933</v>
+        <v>897</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>934</v>
+        <v>898</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>935</v>
+        <v>899</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>936</v>
+        <v>900</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>937</v>
+        <v>901</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>938</v>
+        <v>902</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>939</v>
+        <v>903</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>940</v>
+        <v>904</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>941</v>
+        <v>905</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>942</v>
+        <v>906</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>943</v>
+        <v>907</v>
       </c>
       <c r="O26" s="0" t="s">
-        <v>944</v>
+        <v>908</v>
       </c>
       <c r="P26" s="0" t="s">
-        <v>945</v>
+        <v>909</v>
       </c>
       <c r="Q26" s="0" t="s">
-        <v>946</v>
+        <v>910</v>
       </c>
       <c r="R26" s="0" t="s">
-        <v>947</v>
+        <v>911</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>481</v>
+        <v>446</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>482</v>
+        <v>447</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>948</v>
+        <v>912</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>949</v>
+        <v>913</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>950</v>
+        <v>914</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>951</v>
+        <v>915</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>952</v>
+        <v>916</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>953</v>
+        <v>917</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>954</v>
+        <v>918</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>955</v>
+        <v>919</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>956</v>
+        <v>920</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>957</v>
+        <v>921</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>958</v>
+        <v>922</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>959</v>
+        <v>923</v>
       </c>
       <c r="O27" s="0" t="s">
-        <v>960</v>
+        <v>924</v>
       </c>
       <c r="P27" s="0" t="s">
-        <v>961</v>
+        <v>925</v>
       </c>
       <c r="Q27" s="0" t="s">
-        <v>962</v>
+        <v>926</v>
       </c>
       <c r="R27" s="0" t="s">
-        <v>963</v>
+        <v>927</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>499</v>
+        <v>464</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>500</v>
+        <v>465</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>964</v>
+        <v>928</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>965</v>
+        <v>929</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>966</v>
+        <v>930</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>967</v>
+        <v>931</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>968</v>
+        <v>932</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>969</v>
+        <v>933</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>970</v>
+        <v>934</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>971</v>
+        <v>935</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>972</v>
+        <v>936</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>973</v>
+        <v>937</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>974</v>
+        <v>938</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>975</v>
+        <v>939</v>
       </c>
       <c r="O28" s="0" t="s">
-        <v>976</v>
+        <v>940</v>
       </c>
       <c r="P28" s="0" t="s">
-        <v>977</v>
+        <v>941</v>
       </c>
       <c r="Q28" s="0" t="s">
-        <v>609</v>
+        <v>574</v>
       </c>
       <c r="R28" s="0" t="s">
-        <v>978</v>
+        <v>942</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>517</v>
+        <v>482</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>518</v>
+        <v>483</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>979</v>
+        <v>943</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>980</v>
+        <v>944</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>981</v>
+        <v>945</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>982</v>
+        <v>946</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>983</v>
+        <v>947</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>984</v>
+        <v>948</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>985</v>
+        <v>949</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>982</v>
+        <v>946</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>986</v>
+        <v>950</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>987</v>
+        <v>951</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>988</v>
+        <v>952</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>989</v>
+        <v>953</v>
       </c>
       <c r="O29" s="0" t="s">
-        <v>990</v>
+        <v>954</v>
       </c>
       <c r="P29" s="0" t="s">
-        <v>991</v>
+        <v>955</v>
       </c>
       <c r="Q29" s="0" t="s">
-        <v>992</v>
+        <v>956</v>
       </c>
       <c r="R29" s="0" t="s">
-        <v>993</v>
+        <v>957</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>535</v>
+        <v>500</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>536</v>
+        <v>501</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>994</v>
+        <v>958</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>995</v>
+        <v>959</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>996</v>
+        <v>960</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>997</v>
+        <v>961</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>998</v>
+        <v>962</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>999</v>
+        <v>963</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>1000</v>
+        <v>964</v>
       </c>
       <c r="J30" s="0" t="s">
-        <v>1001</v>
+        <v>965</v>
       </c>
       <c r="K30" s="0" t="s">
-        <v>1002</v>
+        <v>966</v>
       </c>
       <c r="L30" s="0" t="s">
-        <v>1003</v>
+        <v>967</v>
       </c>
       <c r="M30" s="0" t="s">
-        <v>1004</v>
+        <v>968</v>
       </c>
       <c r="N30" s="0" t="s">
-        <v>1005</v>
+        <v>969</v>
       </c>
       <c r="O30" s="0" t="s">
-        <v>1006</v>
+        <v>970</v>
       </c>
       <c r="P30" s="0" t="s">
-        <v>1007</v>
+        <v>971</v>
       </c>
       <c r="Q30" s="0" t="s">
-        <v>1008</v>
+        <v>972</v>
       </c>
       <c r="R30" s="0" t="s">
-        <v>1009</v>
+        <v>973</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>553</v>
+        <v>518</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>554</v>
+        <v>519</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>1010</v>
+        <v>974</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>1011</v>
+        <v>975</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>1012</v>
+        <v>976</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>1013</v>
+        <v>977</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>1014</v>
+        <v>978</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>1015</v>
+        <v>979</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>1016</v>
+        <v>980</v>
       </c>
       <c r="J31" s="0" t="s">
-        <v>1017</v>
+        <v>981</v>
       </c>
       <c r="K31" s="0" t="s">
-        <v>1018</v>
+        <v>982</v>
       </c>
       <c r="L31" s="0" t="s">
-        <v>1019</v>
+        <v>983</v>
       </c>
       <c r="M31" s="0" t="s">
-        <v>1020</v>
+        <v>984</v>
       </c>
       <c r="N31" s="0" t="s">
-        <v>1021</v>
+        <v>985</v>
       </c>
       <c r="O31" s="0" t="s">
-        <v>1022</v>
+        <v>986</v>
       </c>
       <c r="P31" s="0" t="s">
-        <v>1023</v>
+        <v>987</v>
       </c>
       <c r="Q31" s="0" t="s">
-        <v>1024</v>
+        <v>988</v>
       </c>
       <c r="R31" s="0" t="s">
-        <v>1025</v>
+        <v>989</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Decompositions; Clean Output Folder
</commit_message>
<xml_diff>
--- a/out/tab_ex_diff.xlsx
+++ b/out/tab_ex_diff.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="1018">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1012" uniqueCount="1012">
   <si>
     <t xml:space="preserve">region_iso</t>
   </si>
@@ -321,13 +321,13 @@
     <t xml:space="preserve">82.96 (82.86,83.07)</t>
   </si>
   <si>
-    <t xml:space="preserve">76.94 (76.85,77.04)</t>
+    <t xml:space="preserve">76.94 (76.83,77.03)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.91 (-1.07,-0.75)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.36 (-1.50,-1.23)</t>
+    <t xml:space="preserve">-1.36 (-1.52,-1.22)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.16 (+0.11,+0.22)</t>
@@ -342,52 +342,52 @@
     <t xml:space="preserve">Czech Republic</t>
   </si>
   <si>
-    <t xml:space="preserve">81.46 (81.36,81.56)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.64 (75.53,75.74)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.01 (81.91,82.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.16 (76.06,76.26)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.91 (81.82,82.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.12 (76.00,76.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.92 (81.81,82.03)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.20 (76.08,76.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.09 (82.00,82.20)</t>
+    <t xml:space="preserve">81.46 (81.37,81.56)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75.64 (75.52,75.74)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.01 (81.90,82.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.16 (76.05,76.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.91 (81.81,82.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.12 (76.01,76.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.92 (81.81,82.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.20 (76.09,76.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.09 (81.99,82.19)</t>
   </si>
   <si>
     <t xml:space="preserve">76.45 (76.34,76.56)</t>
   </si>
   <si>
-    <t xml:space="preserve">81.18 (81.09,81.27)</t>
+    <t xml:space="preserve">81.18 (81.09,81.28)</t>
   </si>
   <si>
     <t xml:space="preserve">75.34 (75.24,75.45)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.91 (-1.04,-0.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.11 (-1.25,-0.96)</t>
+    <t xml:space="preserve">-0.91 (-1.03,-0.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.11 (-1.26,-0.95)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.16 (+0.12,+0.19)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.20 (+0.17,+0.24)</t>
+    <t xml:space="preserve">+0.20 (+0.16,+0.24)</t>
   </si>
   <si>
     <t xml:space="preserve">DE</t>
@@ -399,10 +399,10 @@
     <t xml:space="preserve">82.93 (82.89,82.96)</t>
   </si>
   <si>
-    <t xml:space="preserve">78.29 (78.25,78.33)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.40 (83.35,83.44)</t>
+    <t xml:space="preserve">78.29 (78.26,78.33)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.40 (83.36,83.43)</t>
   </si>
   <si>
     <t xml:space="preserve">78.64 (78.60,78.69)</t>
@@ -411,7 +411,7 @@
     <t xml:space="preserve">83.40 (83.36,83.44)</t>
   </si>
   <si>
-    <t xml:space="preserve">78.85 (78.80,78.89)</t>
+    <t xml:space="preserve">78.85 (78.81,78.89)</t>
   </si>
   <si>
     <t xml:space="preserve">83.34 (83.30,83.37)</t>
@@ -420,7 +420,7 @@
     <t xml:space="preserve">78.80 (78.76,78.84)</t>
   </si>
   <si>
-    <t xml:space="preserve">83.69 (83.65,83.73)</t>
+    <t xml:space="preserve">83.69 (83.66,83.73)</t>
   </si>
   <si>
     <t xml:space="preserve">79.14 (79.10,79.18)</t>
@@ -429,13 +429,13 @@
     <t xml:space="preserve">83.47 (83.43,83.50)</t>
   </si>
   <si>
-    <t xml:space="preserve">78.80 (78.76,78.83)</t>
+    <t xml:space="preserve">78.80 (78.75,78.83)</t>
   </si>
   <si>
     <t xml:space="preserve">-0.22 (-0.28,-0.17)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.34 (-0.40,-0.29)</t>
+    <t xml:space="preserve">-0.34 (-0.40,-0.28)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.19 (+0.18,+0.20)</t>
@@ -450,52 +450,52 @@
     <t xml:space="preserve">Denmark</t>
   </si>
   <si>
-    <t xml:space="preserve">82.52 (82.37,82.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.72 (78.56,78.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.68 (82.53,82.84)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.95 (78.79,79.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.96 (82.83,83.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.08 (78.92,79.22)</t>
+    <t xml:space="preserve">82.52 (82.35,82.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.72 (78.56,78.85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.68 (82.53,82.83)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.95 (78.79,79.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.96 (82.82,83.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.08 (78.91,79.22)</t>
   </si>
   <si>
     <t xml:space="preserve">82.78 (82.64,82.93)</t>
   </si>
   <si>
-    <t xml:space="preserve">78.96 (78.81,79.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.23 (83.08,83.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.39 (79.25,79.56)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.30 (83.17,83.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.44 (79.31,79.59)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.07 (-0.13,+0.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.05 (-0.17,+0.25)</t>
+    <t xml:space="preserve">78.96 (78.81,79.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.23 (83.08,83.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.39 (79.25,79.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.30 (83.17,83.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.44 (79.29,79.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.07 (-0.11,+0.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.05 (-0.16,+0.27)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.18 (+0.13,+0.23)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.17 (+0.12,+0.22)</t>
+    <t xml:space="preserve">+0.17 (+0.12,+0.23)</t>
   </si>
   <si>
     <t xml:space="preserve">EE</t>
@@ -504,52 +504,52 @@
     <t xml:space="preserve">Estonia</t>
   </si>
   <si>
-    <t xml:space="preserve">81.95 (81.64,82.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.16 (72.81,73.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.11 (81.81,82.40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.33 (72.97,73.65)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.53 (82.23,82.81)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.83 (73.50,74.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.52 (82.25,82.80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.00 (73.70,74.33)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.83 (82.55,83.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.54 (74.21,74.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82.62 (82.34,82.93)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.36 (74.03,74.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.21 (-0.62,+0.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.18 (-0.62,+0.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.22 (+0.12,+0.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.34 (+0.22,+0.46)</t>
+    <t xml:space="preserve">81.95 (81.67,82.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.16 (72.80,73.51)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.11 (81.83,82.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.33 (72.96,73.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.53 (82.23,82.79)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.83 (73.51,74.19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.52 (82.21,82.84)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.00 (73.67,74.31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.83 (82.54,83.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.54 (74.22,74.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82.62 (82.34,82.94)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.36 (74.07,74.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.21 (-0.67,+0.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.18 (-0.64,+0.26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.22 (+0.11,+0.32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.34 (+0.23,+0.46)</t>
   </si>
   <si>
     <t xml:space="preserve">ES</t>
@@ -1251,696 +1251,693 @@
     <t xml:space="preserve">83.88 (83.73,84.02)</t>
   </si>
   <si>
-    <t xml:space="preserve">80.25 (80.09,80.41)</t>
+    <t xml:space="preserve">80.25 (80.09,80.42)</t>
   </si>
   <si>
     <t xml:space="preserve">83.98 (83.83,84.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">80.64 (80.48,80.81)</t>
+    <t xml:space="preserve">80.64 (80.49,80.81)</t>
   </si>
   <si>
     <t xml:space="preserve">84.09 (83.93,84.25)</t>
   </si>
   <si>
-    <t xml:space="preserve">80.90 (80.73,81.07)</t>
+    <t xml:space="preserve">80.90 (80.73,81.06)</t>
   </si>
   <si>
     <t xml:space="preserve">84.26 (84.11,84.40)</t>
   </si>
   <si>
-    <t xml:space="preserve">81.00 (80.86,81.17)</t>
+    <t xml:space="preserve">81.00 (80.85,81.15)</t>
   </si>
   <si>
     <t xml:space="preserve">84.44 (84.30,84.58)</t>
   </si>
   <si>
-    <t xml:space="preserve">81.17 (81.02,81.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.61 (84.46,84.76)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.35 (81.19,81.50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.17 (-0.02,+0.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.18 (-0.03,+0.40)</t>
+    <t xml:space="preserve">81.17 (81.01,81.34)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.61 (84.46,84.75)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.35 (81.21,81.51)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.17 (-0.02,+0.38)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.18 (-0.04,+0.39)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.14 (+0.09,+0.19)</t>
   </si>
   <si>
+    <t xml:space="preserve">+0.23 (+0.18,+0.28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.35 (81.29,81.41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.40 (73.33,73.46)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.89 (81.83,81.95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.85 (73.79,73.91)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.64 (81.58,81.70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.83 (73.76,73.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.66 (81.59,81.72)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.81 (73.74,73.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.96 (81.90,82.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.20 (74.14,74.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.89 (80.83,80.95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72.70 (72.65,72.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.07 (-1.16,-0.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.50 (-1.59,-1.41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.15 (+0.13,+0.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.20 (+0.18,+0.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Portugal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.87 (83.77,83.96)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.03 (77.93,78.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.02 (83.91,84.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.09 (77.98,78.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.29 (84.19,84.39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.41 (78.29,78.53)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.33 (78.20,78.44)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.48 (84.37,84.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.69 (78.58,78.80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.79 (83.69,83.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.86 (77.75,77.97)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.69 (-0.83,-0.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.83 (-0.98,-0.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.15 (+0.12,+0.19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.17 (+0.13,+0.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.89 (76.86,76.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.15 (66.11,66.18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.43 (77.40,77.47)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.91 (66.88,66.95)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.02 (77.99,78.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.84 (67.80,67.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.09 (78.06,78.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.95 (67.92,67.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.44 (78.41,78.47)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68.41 (68.37,68.44)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.64 (76.61,76.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.73 (66.69,66.76)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.80 (-1.85,-1.76)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.68 (-1.72,-1.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.39 (+0.38,+0.40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.56 (+0.55,+0.58)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.14 (80.03,80.26)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.88 (83.77,84.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.47 (80.35,80.58)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.88 (83.77,83.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.59 (80.47,80.70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.00 (83.89,84.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.66 (80.54,80.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.49 (84.39,84.60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.18 (81.07,81.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.90 (83.79,83.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.31 (80.20,80.42)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.59 (-0.74,-0.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.87 (-1.02,-0.71)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.18 (+0.15,+0.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.26 (+0.22,+0.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovenia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.60 (83.38,83.85)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.68 (77.42,77.91)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.04 (83.78,84.29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.15 (77.90,78.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.85 (83.60,84.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.25 (77.98,78.48)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.13 (83.90,84.38)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.47 (78.23,78.73)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84.25 (84.03,84.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78.63 (78.38,78.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83.17 (82.97,83.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77.65 (77.44,77.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.08 (-1.38,-0.80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.98 (-1.33,-0.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.16 (+0.07,+0.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.24 (+0.15,+0.33)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slovakia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.01 (79.85,80.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.00 (72.83,73.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.53 (80.37,80.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.74 (73.57,73.93)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.52 (80.38,80.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.73 (73.57,73.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.56 (80.40,80.71)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.82 (73.66,73.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.92 (80.77,81.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.20 (74.04,74.37)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80.14 (79.99,80.28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73.37 (73.21,73.53)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.79 (-1.01,-0.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.83 (-1.05,-0.59)</t>
+  </si>
+  <si>
     <t xml:space="preserve">+0.23 (+0.17,+0.29)</t>
   </si>
   <si>
-    <t xml:space="preserve">PL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poland</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.35 (81.29,81.42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.40 (73.33,73.46)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.89 (81.84,81.95)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.85 (73.78,73.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.64 (81.58,81.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.83 (73.76,73.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.66 (81.60,81.73)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.81 (73.74,73.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.96 (81.91,82.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.20 (74.14,74.27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.89 (80.83,80.94)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72.70 (72.65,72.76)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.07 (-1.16,-0.98)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.50 (-1.59,-1.41)</t>
+    <t xml:space="preserve">+0.30 (+0.24,+0.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.17 (81.15,81.19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.47 (76.45,76.50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.30 (81.27,81.32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.45 (76.43,76.48)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.29 (81.26,81.31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.43 (76.41,76.45)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.47 (81.45,81.49)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.61 (76.59,76.64)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81.65 (81.63,81.67)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76.74 (76.72,76.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79.99 (79.97,80.01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74.50 (74.47,74.52)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.66 (-1.70,-1.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-2.24 (-2.28,-2.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.12 (+0.11,+0.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.07 (+0.06,+0.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.70 (25.61,25.78)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.26 (22.17,22.37)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.13 (26.04,26.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.69 (22.59,22.79)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.88 (25.79,25.96)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.78 (22.68,22.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.01 (25.92,26.10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.72 (22.62,22.82)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.05 (25.97,26.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.90 (22.79,23.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.38 (25.30,25.46)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.06 (21.97,22.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.67 (-0.79,-0.55)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.84 (-0.97,-0.70)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.09 (+0.06,+0.12)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.46 (25.39,25.55)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.94 (21.84,22.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.00 (25.92,26.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.24 (22.16,22.32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.93 (25.84,26.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.36 (22.27,22.44)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.91 (25.82,25.99)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.50 (22.42,22.59)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.16 (26.08,26.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.79 (22.70,22.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.95 (24.88,25.03)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.56 (21.48,21.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.20 (-1.32,-1.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.23 (-1.34,-1.11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.17 (+0.14,+0.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.21 (+0.18,+0.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.36 (21.28,21.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.97 (16.88,17.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.72 (21.64,21.80)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.24 (17.16,17.33)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.63 (21.56,21.71)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.19 (17.11,17.28)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.79 (21.73,21.87)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.83 (21.75,21.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.20 (17.13,17.29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.71 (20.64,20.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15.80 (15.73,15.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.13 (-1.24,-1.02)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.40 (-1.52,-1.29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.12 (+0.09,+0.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.06 (+0.03,+0.09)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.54 (26.44,26.63)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.33 (23.24,23.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.11 (27.01,27.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.05 (23.94,24.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.04 (26.94,27.15)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.07 (23.97,24.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.11 (27.00,27.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.29 (24.18,24.39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.10 (27.00,27.19)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.40 (24.30,24.49)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.45 (26.38,26.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.50 (23.41,23.60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.64 (-0.76,-0.51)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.89 (-1.03,-0.76)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.14 (+0.11,+0.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.27 (+0.23,+0.30)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.13 (26.02,26.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.15 (22.06,22.25)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.12 (26.02,26.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.48 (26.39,26.60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.58 (22.49,22.66)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.51 (26.41,26.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.63 (22.53,22.72)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.59 (25.50,25.68)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.36 (21.28,21.44)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.92 (-1.05,-0.78)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.27 (-1.40,-1.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.13 (+0.08,+0.18)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.16 (+0.11,+0.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.52 (23.44,23.60)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.36 (19.28,19.43)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.16 (24.07,24.24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.82 (19.73,19.89)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.92 (23.85,24.01)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.80 (19.72,19.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.93 (23.85,24.00)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.90 (19.82,19.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.14 (24.07,24.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20.07 (19.99,20.14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.20 (23.13,23.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.91 (18.84,18.98)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.94 (-1.05,-0.84)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.15 (-1.26,-1.05)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.15 (+0.13,+0.18)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.20 (+0.18,+0.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Portugal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.87 (83.77,83.96)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.03 (77.93,78.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.02 (83.90,84.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.09 (77.98,78.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.29 (84.18,84.38)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.41 (78.29,78.51)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.20 (84.10,84.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.33 (78.21,78.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.48 (84.37,84.59)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.69 (78.57,78.81)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.79 (83.69,83.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.86 (77.76,77.98)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.69 (-0.84,-0.53)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83 (-0.98,-0.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.15 (+0.12,+0.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.17 (+0.13,+0.20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Russia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.89 (76.86,76.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.15 (66.12,66.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.43 (77.40,77.47)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.91 (66.88,66.95)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.02 (77.99,78.05)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.84 (67.80,67.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.09 (78.05,78.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67.95 (67.92,67.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.44 (78.42,78.48)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68.41 (68.37,68.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.64 (76.61,76.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.73 (66.69,66.76)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.80 (-1.85,-1.76)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.68 (-1.72,-1.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.39 (+0.38,+0.40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.56 (+0.55,+0.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sweden</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.76 (83.66,83.86)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.14 (80.03,80.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.88 (83.78,83.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.47 (80.35,80.59)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.88 (83.76,83.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.59 (80.47,80.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.00 (83.88,84.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.66 (80.54,80.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.49 (84.39,84.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.18 (81.06,81.30)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.90 (83.80,83.98)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.31 (80.19,80.42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.59 (-0.76,-0.46)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.87 (-1.03,-0.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.18 (+0.15,+0.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.26 (+0.22,+0.29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovenia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.60 (83.38,83.86)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.68 (77.43,77.93)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.04 (83.79,84.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.15 (77.87,78.42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.85 (83.60,84.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.25 (77.99,78.46)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.13 (83.89,84.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.47 (78.24,78.72)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.25 (84.04,84.47)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78.63 (78.37,78.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83.17 (82.96,83.36)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">77.65 (77.45,77.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.08 (-1.40,-0.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.98 (-1.30,-0.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.16 (+0.08,+0.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.24 (+0.15,+0.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Slovakia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.01 (79.86,80.17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.00 (72.84,73.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.53 (80.37,80.68)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.74 (73.56,73.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.52 (80.37,80.68)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.73 (73.57,73.90)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.56 (80.41,80.70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.82 (73.66,73.97)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.92 (80.77,81.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.20 (74.03,74.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80.14 (79.98,80.26)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73.37 (73.21,73.54)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.79 (-1.02,-0.58)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83 (-1.07,-0.57)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.23 (+0.17,+0.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.30 (+0.24,+0.36)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US</t>
-  </si>
-  <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.17 (81.15,81.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.47 (76.45,76.50)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.30 (81.28,81.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.45 (76.43,76.48)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.29 (81.26,81.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.43 (76.41,76.45)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.47 (81.44,81.49)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.61 (76.59,76.64)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">81.65 (81.62,81.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76.74 (76.72,76.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.99 (79.96,80.01)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74.50 (74.47,74.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.66 (-1.70,-1.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-2.24 (-2.28,-2.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.12 (+0.11,+0.13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.07 (+0.06,+0.08)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.70 (25.61,25.78)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.26 (22.17,22.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.13 (26.04,26.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.69 (22.59,22.79)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.88 (25.79,25.96)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.78 (22.68,22.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.01 (25.92,26.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.72 (22.62,22.82)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.05 (25.97,26.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.90 (22.79,23.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.38 (25.30,25.46)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.06 (21.97,22.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.67 (-0.79,-0.55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.84 (-0.97,-0.70)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.09 (+0.06,+0.12)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.46 (25.39,25.55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.94 (21.84,22.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.00 (25.92,26.09)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.24 (22.16,22.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.93 (25.84,26.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.36 (22.27,22.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.91 (25.82,25.99)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.50 (22.42,22.59)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.16 (26.08,26.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.79 (22.70,22.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.95 (24.88,25.03)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.56 (21.48,21.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.20 (-1.32,-1.09)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.23 (-1.34,-1.11)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.17 (+0.14,+0.20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.21 (+0.18,+0.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.36 (21.28,21.43)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.97 (16.88,17.04)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.72 (21.64,21.80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.24 (17.16,17.33)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.63 (21.56,21.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.19 (17.11,17.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.79 (21.73,21.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.83 (21.75,21.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17.20 (17.13,17.29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.71 (20.64,20.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15.80 (15.73,15.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.13 (-1.24,-1.02)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.40 (-1.52,-1.29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.12 (+0.09,+0.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.06 (+0.03,+0.09)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.54 (26.44,26.63)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.33 (23.24,23.43)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.11 (27.01,27.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.05 (23.94,24.16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.04 (26.94,27.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.07 (23.97,24.16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.11 (27.00,27.20)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.29 (24.18,24.39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27.10 (27.00,27.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.40 (24.30,24.49)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.45 (26.38,26.54)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.50 (23.41,23.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.64 (-0.76,-0.51)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.89 (-1.03,-0.76)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.14 (+0.11,+0.17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.27 (+0.23,+0.30)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.13 (26.02,26.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.15 (22.06,22.25)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.12 (26.02,26.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.48 (26.39,26.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.58 (22.49,22.66)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.51 (26.41,26.61)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.63 (22.53,22.72)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.59 (25.50,25.68)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.36 (21.28,21.44)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.92 (-1.05,-0.78)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.27 (-1.40,-1.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.13 (+0.08,+0.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.16 (+0.11,+0.21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.52 (23.44,23.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.36 (19.28,19.43)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.16 (24.07,24.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.82 (19.73,19.89)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.92 (23.85,24.01)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.80 (19.72,19.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.93 (23.85,24.00)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.90 (19.82,19.97)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.14 (24.07,24.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20.07 (19.99,20.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.20 (23.14,23.27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.91 (18.84,18.98)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.94 (-1.05,-0.84)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.15 (-1.26,-1.05)</t>
-  </si>
-  <si>
     <t xml:space="preserve">+0.18 (+0.15,+0.20)</t>
   </si>
   <si>
@@ -1965,7 +1962,7 @@
     <t xml:space="preserve">25.34 (25.31,25.37)</t>
   </si>
   <si>
-    <t xml:space="preserve">21.97 (21.94,22.00)</t>
+    <t xml:space="preserve">21.97 (21.93,22.00)</t>
   </si>
   <si>
     <t xml:space="preserve">25.64 (25.61,25.67)</t>
@@ -1986,100 +1983,97 @@
     <t xml:space="preserve">-0.38 (-0.42,-0.34)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.16 (+0.16,+0.17)</t>
-  </si>
-  <si>
     <t xml:space="preserve">+0.16 (+0.15,+0.17)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.64 (24.52,24.77)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.77 (21.65,21.87)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.79 (24.67,24.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.03 (21.92,22.15)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.95 (24.84,25.08)</t>
+    <t xml:space="preserve">24.64 (24.52,24.76)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.77 (21.64,21.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.79 (24.68,24.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.03 (21.91,22.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.95 (24.83,25.07)</t>
   </si>
   <si>
     <t xml:space="preserve">22.08 (21.95,22.19)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.76 (24.64,24.88)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.92 (21.82,22.03)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.05 (24.95,25.16)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.16 (22.05,22.27)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.11 (25.00,25.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.18 (22.08,22.29)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.06 (-0.10,+0.23)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.01 (-0.13,+0.16)</t>
+    <t xml:space="preserve">24.76 (24.66,24.88)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.92 (21.81,22.04)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.05 (24.94,25.16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.16 (22.04,22.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.11 (25.00,25.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.18 (22.06,22.29)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.06 (-0.09,+0.22)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.01 (-0.14,+0.18)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.10 (+0.06,+0.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.57 (24.36,24.78)</t>
+    <t xml:space="preserve">24.57 (24.38,24.78)</t>
   </si>
   <si>
     <t xml:space="preserve">18.66 (18.40,18.91)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.88 (24.67,25.09)</t>
+    <t xml:space="preserve">24.88 (24.66,25.09)</t>
   </si>
   <si>
     <t xml:space="preserve">18.78 (18.53,19.04)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.85 (24.63,25.07)</t>
+    <t xml:space="preserve">24.85 (24.64,25.05)</t>
   </si>
   <si>
     <t xml:space="preserve">18.85 (18.62,19.14)</t>
   </si>
   <si>
-    <t xml:space="preserve">24.74 (24.54,24.96)</t>
+    <t xml:space="preserve">24.74 (24.53,24.96)</t>
   </si>
   <si>
     <t xml:space="preserve">18.99 (18.74,19.24)</t>
   </si>
   <si>
-    <t xml:space="preserve">25.19 (24.99,25.42)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19.26 (19.02,19.49)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24.98 (24.79,25.20)</t>
+    <t xml:space="preserve">25.19 (24.98,25.42)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19.26 (19.02,19.50)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24.98 (24.78,25.19)</t>
   </si>
   <si>
     <t xml:space="preserve">19.14 (18.90,19.37)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.20 (-0.52,+0.10)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.12 (-0.46,+0.18)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.15 (+0.08,+0.24)</t>
+    <t xml:space="preserve">-0.20 (-0.52,+0.08)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.12 (-0.46,+0.21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.15 (+0.07,+0.24)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.15 (+0.06,+0.24)</t>
@@ -2715,25 +2709,25 @@
     <t xml:space="preserve">25.88 (25.75,26.00)</t>
   </si>
   <si>
-    <t xml:space="preserve">23.48 (23.35,23.60)</t>
+    <t xml:space="preserve">23.48 (23.37,23.61)</t>
   </si>
   <si>
     <t xml:space="preserve">26.03 (25.91,26.16)</t>
   </si>
   <si>
-    <t xml:space="preserve">23.61 (23.47,23.72)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.18 (26.06,26.32)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.72 (23.60,23.84)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.15 (-0.02,+0.34)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.11 (-0.07,+0.29)</t>
+    <t xml:space="preserve">23.61 (23.48,23.73)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.18 (26.05,26.32)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.72 (23.59,23.83)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.15 (-0.01,+0.34)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.11 (-0.06,+0.27)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.10 (+0.06,+0.15)</t>
@@ -2772,13 +2766,13 @@
     <t xml:space="preserve">23.33 (23.29,23.37)</t>
   </si>
   <si>
-    <t xml:space="preserve">17.89 (17.86,17.93)</t>
+    <t xml:space="preserve">17.89 (17.85,17.93)</t>
   </si>
   <si>
     <t xml:space="preserve">-1.12 (-1.19,-1.06)</t>
   </si>
   <si>
-    <t xml:space="preserve">-1.53 (-1.60,-1.48)</t>
+    <t xml:space="preserve">-1.53 (-1.60,-1.47)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.13 (+0.12,+0.15)</t>
@@ -2790,7 +2784,7 @@
     <t xml:space="preserve">25.73 (25.66,25.80)</t>
   </si>
   <si>
-    <t xml:space="preserve">21.80 (21.72,21.88)</t>
+    <t xml:space="preserve">21.80 (21.71,21.88)</t>
   </si>
   <si>
     <t xml:space="preserve">25.96 (25.89,26.03)</t>
@@ -2802,34 +2796,34 @@
     <t xml:space="preserve">26.26 (26.17,26.33)</t>
   </si>
   <si>
-    <t xml:space="preserve">22.12 (22.04,22.20)</t>
+    <t xml:space="preserve">22.12 (22.04,22.21)</t>
   </si>
   <si>
     <t xml:space="preserve">26.22 (26.15,26.29)</t>
   </si>
   <si>
-    <t xml:space="preserve">21.99 (21.90,22.06)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.48 (26.40,26.57)</t>
+    <t xml:space="preserve">21.99 (21.90,22.07)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.48 (26.41,26.57)</t>
   </si>
   <si>
     <t xml:space="preserve">22.21 (22.12,22.29)</t>
   </si>
   <si>
-    <t xml:space="preserve">25.76 (25.70,25.83)</t>
+    <t xml:space="preserve">25.76 (25.69,25.84)</t>
   </si>
   <si>
     <t xml:space="preserve">21.50 (21.42,21.58)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.72 (-0.83,-0.61)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.71 (-0.82,-0.60)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.19 (+0.16,+0.21)</t>
+    <t xml:space="preserve">-0.72 (-0.82,-0.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.71 (-0.83,-0.61)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+0.19 (+0.16,+0.22)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.10 (+0.07,+0.13)</t>
@@ -2859,16 +2853,16 @@
     <t xml:space="preserve">16.59 (16.56,16.61)</t>
   </si>
   <si>
-    <t xml:space="preserve">22.53 (22.51,22.55)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16.84 (16.82,16.87)</t>
+    <t xml:space="preserve">22.53 (22.50,22.55)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.84 (16.81,16.87)</t>
   </si>
   <si>
     <t xml:space="preserve">20.98 (20.96,20.99)</t>
   </si>
   <si>
-    <t xml:space="preserve">15.19 (15.18,15.22)</t>
+    <t xml:space="preserve">15.19 (15.17,15.22)</t>
   </si>
   <si>
     <t xml:space="preserve">-1.55 (-1.58,-1.52)</t>
@@ -2883,16 +2877,16 @@
     <t xml:space="preserve">+0.20 (+0.19,+0.21)</t>
   </si>
   <si>
-    <t xml:space="preserve">25.49 (25.41,25.57)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.84 (22.75,22.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.63 (25.56,25.71)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.07 (22.97,23.16)</t>
+    <t xml:space="preserve">25.49 (25.41,25.58)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22.84 (22.76,22.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.63 (25.55,25.72)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.07 (22.98,23.15)</t>
   </si>
   <si>
     <t xml:space="preserve">25.60 (25.52,25.69)</t>
@@ -2901,121 +2895,109 @@
     <t xml:space="preserve">23.20 (23.11,23.28)</t>
   </si>
   <si>
-    <t xml:space="preserve">25.70 (25.61,25.79)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.22 (23.14,23.31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26.17 (26.09,26.25)</t>
+    <t xml:space="preserve">25.70 (25.62,25.78)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.22 (23.15,23.31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26.17 (26.08,26.27)</t>
   </si>
   <si>
     <t xml:space="preserve">23.60 (23.52,23.68)</t>
   </si>
   <si>
-    <t xml:space="preserve">25.51 (25.43,25.58)</t>
+    <t xml:space="preserve">25.51 (25.43,25.57)</t>
   </si>
   <si>
     <t xml:space="preserve">22.81 (22.73,22.89)</t>
   </si>
   <si>
-    <t xml:space="preserve">-0.66 (-0.78,-0.56)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.80 (-0.91,-0.67)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+0.19 (+0.16,+0.22)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.44 (25.27,25.65)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.17 (20.96,21.37)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.87 (25.68,26.06)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.57 (21.38,21.80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.72 (25.54,25.91)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.33 (21.14,21.52)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25.86 (25.67,26.06)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21.57 (21.38,21.75)</t>
+    <t xml:space="preserve">-0.66 (-0.78,-0.54)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.80 (-0.92,-0.68)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.44 (25.25,25.62)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.17 (20.96,21.36)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.87 (25.68,26.07)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.57 (21.38,21.79)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.72 (25.54,25.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.33 (21.13,21.51)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25.86 (25.68,26.05)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.57 (21.37,21.77)</t>
   </si>
   <si>
     <t xml:space="preserve">25.83 (25.66,26.01)</t>
   </si>
   <si>
-    <t xml:space="preserve">21.83 (21.63,22.03)</t>
+    <t xml:space="preserve">21.83 (21.64,22.02)</t>
   </si>
   <si>
     <t xml:space="preserve">24.80 (24.65,24.95)</t>
   </si>
   <si>
-    <t xml:space="preserve">20.72 (20.56,20.92)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.03 (-1.26,-0.80)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-1.10 (-1.39,-0.85)</t>
+    <t xml:space="preserve">20.72 (20.57,20.92)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.03 (-1.25,-0.77)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.10 (-1.34,-0.83)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.10 (+0.03,+0.16)</t>
   </si>
   <si>
-    <t xml:space="preserve">+0.16 (+0.09,+0.24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22.65 (22.54,22.74)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.08 (17.96,18.19)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.14 (23.03,23.24)</t>
+    <t xml:space="preserve">+0.16 (+0.10,+0.23)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.08 (17.97,18.20)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.14 (23.03,23.25)</t>
   </si>
   <si>
     <t xml:space="preserve">18.49 (18.36,18.61)</t>
   </si>
   <si>
-    <t xml:space="preserve">23.06 (22.95,23.17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.49 (18.37,18.61)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.16 (23.04,23.28)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.69 (18.59,18.81)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23.53 (23.42,23.65)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18.92 (18.80,19.05)</t>
+    <t xml:space="preserve">23.06 (22.96,23.17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.16 (23.05,23.27)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.69 (18.57,18.81)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.53 (23.41,23.64)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.92 (18.78,19.04)</t>
   </si>
   <si>
     <t xml:space="preserve">22.70 (22.61,22.81)</t>
   </si>
   <si>
-    <t xml:space="preserve">18.03 (17.92,18.14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.83 (-0.97,-0.68)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-0.89 (-1.06,-0.73)</t>
+    <t xml:space="preserve">18.03 (17.94,18.13)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-0.89 (-1.04,-0.72)</t>
   </si>
   <si>
     <t xml:space="preserve">+0.22 (+0.18,+0.26)</t>
@@ -3024,13 +3006,13 @@
     <t xml:space="preserve">24.75 (24.73,24.77)</t>
   </si>
   <si>
-    <t xml:space="preserve">21.87 (21.86,21.89)</t>
+    <t xml:space="preserve">21.87 (21.85,21.89)</t>
   </si>
   <si>
     <t xml:space="preserve">24.98 (24.96,24.99)</t>
   </si>
   <si>
-    <t xml:space="preserve">22.08 (22.06,22.09)</t>
+    <t xml:space="preserve">22.08 (22.06,22.10)</t>
   </si>
   <si>
     <t xml:space="preserve">24.92 (24.90,24.94)</t>
@@ -4824,314 +4806,314 @@
         <v>452</v>
       </c>
       <c r="I26" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" t="s">
         <v>453</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>454</v>
       </c>
-      <c r="K26" t="s">
+      <c r="L26" t="s">
         <v>455</v>
       </c>
-      <c r="L26" t="s">
+      <c r="M26" t="s">
         <v>456</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>457</v>
       </c>
-      <c r="N26" t="s">
+      <c r="O26" t="s">
         <v>458</v>
       </c>
-      <c r="O26" t="s">
+      <c r="P26" t="s">
         <v>459</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" t="s">
         <v>460</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>461</v>
-      </c>
-      <c r="R26" t="s">
-        <v>462</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B27" t="s">
         <v>463</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>464</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>465</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>466</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>467</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>468</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>469</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>470</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>471</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>472</v>
       </c>
-      <c r="K27" t="s">
+      <c r="L27" t="s">
         <v>473</v>
       </c>
-      <c r="L27" t="s">
+      <c r="M27" t="s">
         <v>474</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>475</v>
       </c>
-      <c r="N27" t="s">
+      <c r="O27" t="s">
         <v>476</v>
       </c>
-      <c r="O27" t="s">
+      <c r="P27" t="s">
         <v>477</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" t="s">
         <v>478</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>479</v>
-      </c>
-      <c r="R27" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>480</v>
+      </c>
+      <c r="B28" t="s">
         <v>481</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>44</v>
+      </c>
+      <c r="D28" t="s">
         <v>482</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>483</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>484</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>485</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>486</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>487</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>488</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>489</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>490</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>491</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>492</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>493</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>494</v>
       </c>
-      <c r="O28" t="s">
+      <c r="Q28" t="s">
         <v>495</v>
       </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
         <v>496</v>
-      </c>
-      <c r="Q28" t="s">
-        <v>497</v>
-      </c>
-      <c r="R28" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>497</v>
+      </c>
+      <c r="B29" t="s">
+        <v>498</v>
+      </c>
+      <c r="C29" t="s">
         <v>499</v>
       </c>
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>500</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>501</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>502</v>
       </c>
-      <c r="E29" t="s">
+      <c r="G29" t="s">
         <v>503</v>
       </c>
-      <c r="F29" t="s">
+      <c r="H29" t="s">
         <v>504</v>
       </c>
-      <c r="G29" t="s">
+      <c r="I29" t="s">
         <v>505</v>
       </c>
-      <c r="H29" t="s">
+      <c r="J29" t="s">
         <v>506</v>
       </c>
-      <c r="I29" t="s">
+      <c r="K29" t="s">
         <v>507</v>
       </c>
-      <c r="J29" t="s">
+      <c r="L29" t="s">
         <v>508</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>509</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>510</v>
       </c>
-      <c r="M29" t="s">
+      <c r="O29" t="s">
         <v>511</v>
       </c>
-      <c r="N29" t="s">
+      <c r="P29" t="s">
         <v>512</v>
       </c>
-      <c r="O29" t="s">
+      <c r="Q29" t="s">
         <v>513</v>
       </c>
-      <c r="P29" t="s">
+      <c r="R29" t="s">
         <v>514</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>515</v>
-      </c>
-      <c r="R29" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>515</v>
+      </c>
+      <c r="B30" t="s">
+        <v>516</v>
+      </c>
+      <c r="C30" t="s">
         <v>517</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30" t="s">
         <v>518</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>519</v>
       </c>
-      <c r="D30" t="s">
+      <c r="F30" t="s">
         <v>520</v>
       </c>
-      <c r="E30" t="s">
+      <c r="G30" t="s">
         <v>521</v>
       </c>
-      <c r="F30" t="s">
+      <c r="H30" t="s">
         <v>522</v>
       </c>
-      <c r="G30" t="s">
+      <c r="I30" t="s">
         <v>523</v>
       </c>
-      <c r="H30" t="s">
+      <c r="J30" t="s">
         <v>524</v>
       </c>
-      <c r="I30" t="s">
+      <c r="K30" t="s">
         <v>525</v>
       </c>
-      <c r="J30" t="s">
+      <c r="L30" t="s">
         <v>526</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>527</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>528</v>
       </c>
-      <c r="M30" t="s">
+      <c r="O30" t="s">
         <v>529</v>
       </c>
-      <c r="N30" t="s">
+      <c r="P30" t="s">
         <v>530</v>
       </c>
-      <c r="O30" t="s">
+      <c r="Q30" t="s">
         <v>531</v>
       </c>
-      <c r="P30" t="s">
+      <c r="R30" t="s">
         <v>532</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>533</v>
-      </c>
-      <c r="R30" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
+        <v>533</v>
+      </c>
+      <c r="B31" t="s">
+        <v>534</v>
+      </c>
+      <c r="C31" t="s">
         <v>535</v>
       </c>
-      <c r="B31" t="s">
+      <c r="D31" t="s">
         <v>536</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>537</v>
       </c>
-      <c r="D31" t="s">
+      <c r="F31" t="s">
         <v>538</v>
       </c>
-      <c r="E31" t="s">
+      <c r="G31" t="s">
         <v>539</v>
       </c>
-      <c r="F31" t="s">
+      <c r="H31" t="s">
         <v>540</v>
       </c>
-      <c r="G31" t="s">
+      <c r="I31" t="s">
         <v>541</v>
       </c>
-      <c r="H31" t="s">
+      <c r="J31" t="s">
         <v>542</v>
       </c>
-      <c r="I31" t="s">
+      <c r="K31" t="s">
         <v>543</v>
       </c>
-      <c r="J31" t="s">
+      <c r="L31" t="s">
         <v>544</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>545</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>546</v>
       </c>
-      <c r="M31" t="s">
+      <c r="O31" t="s">
         <v>547</v>
       </c>
-      <c r="N31" t="s">
+      <c r="P31" t="s">
         <v>548</v>
       </c>
-      <c r="O31" t="s">
+      <c r="Q31" t="s">
         <v>549</v>
       </c>
-      <c r="P31" t="s">
+      <c r="R31" t="s">
         <v>550</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>551</v>
-      </c>
-      <c r="R31" t="s">
-        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -5212,49 +5194,49 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
+        <v>551</v>
+      </c>
+      <c r="D2" t="s">
+        <v>552</v>
+      </c>
+      <c r="E2" t="s">
         <v>553</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>554</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>555</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>556</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>557</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>558</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>559</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>560</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>561</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" t="s">
         <v>562</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>563</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>564</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>565</v>
-      </c>
-      <c r="P2" t="s">
-        <v>566</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>567</v>
       </c>
       <c r="R2" t="s">
         <v>123</v>
@@ -5268,52 +5250,52 @@
         <v>37</v>
       </c>
       <c r="C3" t="s">
+        <v>566</v>
+      </c>
+      <c r="D3" t="s">
+        <v>567</v>
+      </c>
+      <c r="E3" t="s">
         <v>568</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>569</v>
       </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
         <v>570</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>571</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>572</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>573</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>574</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>575</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>576</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>577</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>578</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>579</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>580</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>581</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>582</v>
-      </c>
-      <c r="R3" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="4">
@@ -5324,52 +5306,52 @@
         <v>55</v>
       </c>
       <c r="C4" t="s">
+        <v>582</v>
+      </c>
+      <c r="D4" t="s">
+        <v>583</v>
+      </c>
+      <c r="E4" t="s">
         <v>584</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>585</v>
       </c>
-      <c r="E4" t="s">
+      <c r="G4" t="s">
         <v>586</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
         <v>587</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>588</v>
       </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
+        <v>585</v>
+      </c>
+      <c r="K4" t="s">
         <v>589</v>
       </c>
-      <c r="I4" t="s">
+      <c r="L4" t="s">
         <v>590</v>
       </c>
-      <c r="J4" t="s">
-        <v>587</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>591</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>592</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>593</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>594</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>595</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>596</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>597</v>
-      </c>
-      <c r="R4" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="5">
@@ -5380,52 +5362,52 @@
         <v>73</v>
       </c>
       <c r="C5" t="s">
+        <v>597</v>
+      </c>
+      <c r="D5" t="s">
+        <v>598</v>
+      </c>
+      <c r="E5" t="s">
         <v>599</v>
       </c>
-      <c r="D5" t="s">
+      <c r="F5" t="s">
         <v>600</v>
       </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
         <v>601</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>602</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>603</v>
       </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>604</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>605</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>606</v>
       </c>
-      <c r="K5" t="s">
+      <c r="M5" t="s">
         <v>607</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>608</v>
       </c>
-      <c r="M5" t="s">
+      <c r="O5" t="s">
         <v>609</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>610</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>611</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>612</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>613</v>
-      </c>
-      <c r="R5" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="6">
@@ -5442,46 +5424,46 @@
         <v>92</v>
       </c>
       <c r="E6" t="s">
+        <v>613</v>
+      </c>
+      <c r="F6" t="s">
+        <v>614</v>
+      </c>
+      <c r="G6" t="s">
         <v>615</v>
       </c>
-      <c r="F6" t="s">
+      <c r="H6" t="s">
+        <v>552</v>
+      </c>
+      <c r="I6" t="s">
         <v>616</v>
       </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>617</v>
       </c>
-      <c r="H6" t="s">
-        <v>554</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>618</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>619</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>620</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>621</v>
       </c>
-      <c r="M6" t="s">
+      <c r="O6" t="s">
         <v>622</v>
       </c>
-      <c r="N6" t="s">
+      <c r="P6" t="s">
         <v>623</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>624</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>625</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>626</v>
-      </c>
-      <c r="R6" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="7">
@@ -5492,52 +5474,52 @@
         <v>108</v>
       </c>
       <c r="C7" t="s">
+        <v>626</v>
+      </c>
+      <c r="D7" t="s">
+        <v>627</v>
+      </c>
+      <c r="E7" t="s">
         <v>628</v>
       </c>
-      <c r="D7" t="s">
+      <c r="F7" t="s">
         <v>629</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>630</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>631</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>632</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>633</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>634</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>635</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>636</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>637</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
         <v>638</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" t="s">
         <v>639</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>640</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>641</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>443</v>
-      </c>
-      <c r="R7" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="8">
@@ -5548,52 +5530,52 @@
         <v>126</v>
       </c>
       <c r="C8" t="s">
+        <v>642</v>
+      </c>
+      <c r="D8" t="s">
         <v>643</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>644</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>645</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>646</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>647</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>648</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>649</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>650</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>651</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>652</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>653</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>654</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>655</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>656</v>
       </c>
-      <c r="Q8" t="s">
-        <v>657</v>
-      </c>
       <c r="R8" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="9">
@@ -5604,52 +5586,52 @@
         <v>144</v>
       </c>
       <c r="C9" t="s">
+        <v>657</v>
+      </c>
+      <c r="D9" t="s">
+        <v>658</v>
+      </c>
+      <c r="E9" t="s">
         <v>659</v>
       </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>660</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>661</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>662</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>663</v>
       </c>
-      <c r="H9" t="s">
+      <c r="J9" t="s">
         <v>664</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>665</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>666</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>667</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>668</v>
       </c>
-      <c r="M9" t="s">
+      <c r="O9" t="s">
         <v>669</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>670</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>671</v>
       </c>
-      <c r="P9" t="s">
-        <v>672</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>673</v>
-      </c>
       <c r="R9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="10">
@@ -5660,52 +5642,52 @@
         <v>162</v>
       </c>
       <c r="C10" t="s">
+        <v>672</v>
+      </c>
+      <c r="D10" t="s">
+        <v>673</v>
+      </c>
+      <c r="E10" t="s">
         <v>674</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>675</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>676</v>
       </c>
-      <c r="F10" t="s">
+      <c r="H10" t="s">
         <v>677</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>678</v>
       </c>
-      <c r="H10" t="s">
+      <c r="J10" t="s">
         <v>679</v>
       </c>
-      <c r="I10" t="s">
+      <c r="K10" t="s">
         <v>680</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>681</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>682</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>683</v>
       </c>
-      <c r="M10" t="s">
+      <c r="O10" t="s">
         <v>684</v>
       </c>
-      <c r="N10" t="s">
+      <c r="P10" t="s">
         <v>685</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>686</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>687</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>688</v>
-      </c>
-      <c r="R10" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="11">
@@ -5716,52 +5698,52 @@
         <v>180</v>
       </c>
       <c r="C11" t="s">
+        <v>688</v>
+      </c>
+      <c r="D11" t="s">
+        <v>689</v>
+      </c>
+      <c r="E11" t="s">
         <v>690</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>691</v>
       </c>
-      <c r="E11" t="s">
+      <c r="G11" t="s">
         <v>692</v>
       </c>
-      <c r="F11" t="s">
+      <c r="H11" t="s">
         <v>693</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>694</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>695</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>696</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>697</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>698</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>699</v>
       </c>
-      <c r="M11" t="s">
+      <c r="O11" t="s">
         <v>700</v>
       </c>
-      <c r="N11" t="s">
+      <c r="P11" t="s">
         <v>701</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>702</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>703</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>704</v>
-      </c>
-      <c r="R11" t="s">
-        <v>705</v>
       </c>
     </row>
     <row r="12">
@@ -5772,52 +5754,52 @@
         <v>198</v>
       </c>
       <c r="C12" t="s">
+        <v>704</v>
+      </c>
+      <c r="D12" t="s">
+        <v>705</v>
+      </c>
+      <c r="E12" t="s">
         <v>706</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>707</v>
       </c>
-      <c r="E12" t="s">
+      <c r="G12" t="s">
         <v>708</v>
       </c>
-      <c r="F12" t="s">
+      <c r="H12" t="s">
         <v>709</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>710</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>711</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>712</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>713</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>714</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>715</v>
       </c>
-      <c r="M12" t="s">
+      <c r="O12" t="s">
         <v>716</v>
       </c>
-      <c r="N12" t="s">
+      <c r="P12" t="s">
         <v>717</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>718</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>719</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>720</v>
-      </c>
-      <c r="R12" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="13">
@@ -5828,52 +5810,52 @@
         <v>216</v>
       </c>
       <c r="C13" t="s">
+        <v>720</v>
+      </c>
+      <c r="D13" t="s">
+        <v>721</v>
+      </c>
+      <c r="E13" t="s">
         <v>722</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>723</v>
       </c>
-      <c r="E13" t="s">
+      <c r="G13" t="s">
         <v>724</v>
       </c>
-      <c r="F13" t="s">
+      <c r="H13" t="s">
         <v>725</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>726</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>727</v>
       </c>
-      <c r="I13" t="s">
+      <c r="K13" t="s">
         <v>728</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>729</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>730</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>731</v>
       </c>
-      <c r="M13" t="s">
+      <c r="O13" t="s">
         <v>732</v>
       </c>
-      <c r="N13" t="s">
+      <c r="P13" t="s">
         <v>733</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>734</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>735</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>736</v>
-      </c>
-      <c r="R13" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="14">
@@ -5884,52 +5866,52 @@
         <v>234</v>
       </c>
       <c r="C14" t="s">
+        <v>736</v>
+      </c>
+      <c r="D14" t="s">
+        <v>737</v>
+      </c>
+      <c r="E14" t="s">
         <v>738</v>
       </c>
-      <c r="D14" t="s">
+      <c r="F14" t="s">
         <v>739</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>740</v>
       </c>
-      <c r="F14" t="s">
+      <c r="H14" t="s">
         <v>741</v>
       </c>
-      <c r="G14" t="s">
+      <c r="I14" t="s">
         <v>742</v>
       </c>
-      <c r="H14" t="s">
+      <c r="J14" t="s">
         <v>743</v>
       </c>
-      <c r="I14" t="s">
+      <c r="K14" t="s">
         <v>744</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>745</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>746</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>747</v>
       </c>
-      <c r="M14" t="s">
+      <c r="O14" t="s">
         <v>748</v>
       </c>
-      <c r="N14" t="s">
+      <c r="P14" t="s">
         <v>749</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>750</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>751</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>752</v>
-      </c>
-      <c r="R14" t="s">
-        <v>753</v>
       </c>
     </row>
     <row r="15">
@@ -5940,52 +5922,52 @@
         <v>252</v>
       </c>
       <c r="C15" t="s">
+        <v>752</v>
+      </c>
+      <c r="D15" t="s">
+        <v>753</v>
+      </c>
+      <c r="E15" t="s">
         <v>754</v>
       </c>
-      <c r="D15" t="s">
+      <c r="F15" t="s">
         <v>755</v>
       </c>
-      <c r="E15" t="s">
+      <c r="G15" t="s">
         <v>756</v>
       </c>
-      <c r="F15" t="s">
+      <c r="H15" t="s">
         <v>757</v>
       </c>
-      <c r="G15" t="s">
+      <c r="I15" t="s">
         <v>758</v>
       </c>
-      <c r="H15" t="s">
+      <c r="J15" t="s">
         <v>759</v>
       </c>
-      <c r="I15" t="s">
+      <c r="K15" t="s">
         <v>760</v>
       </c>
-      <c r="J15" t="s">
+      <c r="L15" t="s">
         <v>761</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>762</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>763</v>
       </c>
-      <c r="M15" t="s">
+      <c r="O15" t="s">
         <v>764</v>
       </c>
-      <c r="N15" t="s">
+      <c r="P15" t="s">
         <v>765</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>766</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>767</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>768</v>
-      </c>
-      <c r="R15" t="s">
-        <v>769</v>
       </c>
     </row>
     <row r="16">
@@ -5996,52 +5978,52 @@
         <v>270</v>
       </c>
       <c r="C16" t="s">
+        <v>768</v>
+      </c>
+      <c r="D16" t="s">
+        <v>769</v>
+      </c>
+      <c r="E16" t="s">
         <v>770</v>
       </c>
-      <c r="D16" t="s">
+      <c r="F16" t="s">
         <v>771</v>
       </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>772</v>
       </c>
-      <c r="F16" t="s">
+      <c r="H16" t="s">
         <v>773</v>
       </c>
-      <c r="G16" t="s">
+      <c r="I16" t="s">
         <v>774</v>
       </c>
-      <c r="H16" t="s">
+      <c r="J16" t="s">
         <v>775</v>
       </c>
-      <c r="I16" t="s">
+      <c r="K16" t="s">
         <v>776</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>777</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>778</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>779</v>
       </c>
-      <c r="M16" t="s">
+      <c r="O16" t="s">
         <v>780</v>
       </c>
-      <c r="N16" t="s">
+      <c r="P16" t="s">
         <v>781</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>782</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>783</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>784</v>
-      </c>
-      <c r="R16" t="s">
-        <v>785</v>
       </c>
     </row>
     <row r="17">
@@ -6058,46 +6040,46 @@
         <v>92</v>
       </c>
       <c r="E17" t="s">
+        <v>784</v>
+      </c>
+      <c r="F17" t="s">
+        <v>785</v>
+      </c>
+      <c r="G17" t="s">
         <v>786</v>
       </c>
-      <c r="F17" t="s">
+      <c r="H17" t="s">
         <v>787</v>
       </c>
-      <c r="G17" t="s">
+      <c r="I17" t="s">
         <v>788</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>789</v>
       </c>
-      <c r="I17" t="s">
+      <c r="K17" t="s">
         <v>790</v>
       </c>
-      <c r="J17" t="s">
+      <c r="L17" t="s">
         <v>791</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>792</v>
       </c>
-      <c r="L17" t="s">
+      <c r="N17" t="s">
         <v>793</v>
       </c>
-      <c r="M17" t="s">
+      <c r="O17" t="s">
         <v>794</v>
       </c>
-      <c r="N17" t="s">
+      <c r="P17" t="s">
         <v>795</v>
       </c>
-      <c r="O17" t="s">
+      <c r="Q17" t="s">
         <v>796</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>797</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>798</v>
-      </c>
-      <c r="R17" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="18">
@@ -6108,52 +6090,52 @@
         <v>304</v>
       </c>
       <c r="C18" t="s">
+        <v>798</v>
+      </c>
+      <c r="D18" t="s">
+        <v>799</v>
+      </c>
+      <c r="E18" t="s">
         <v>800</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>801</v>
       </c>
-      <c r="E18" t="s">
+      <c r="G18" t="s">
         <v>802</v>
       </c>
-      <c r="F18" t="s">
+      <c r="H18" t="s">
         <v>803</v>
       </c>
-      <c r="G18" t="s">
+      <c r="I18" t="s">
         <v>804</v>
       </c>
-      <c r="H18" t="s">
+      <c r="J18" t="s">
         <v>805</v>
       </c>
-      <c r="I18" t="s">
+      <c r="K18" t="s">
         <v>806</v>
       </c>
-      <c r="J18" t="s">
+      <c r="L18" t="s">
         <v>807</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>808</v>
       </c>
-      <c r="L18" t="s">
+      <c r="N18" t="s">
         <v>809</v>
       </c>
-      <c r="M18" t="s">
+      <c r="O18" t="s">
         <v>810</v>
       </c>
-      <c r="N18" t="s">
+      <c r="P18" t="s">
         <v>811</v>
       </c>
-      <c r="O18" t="s">
+      <c r="Q18" t="s">
+        <v>783</v>
+      </c>
+      <c r="R18" t="s">
         <v>812</v>
-      </c>
-      <c r="P18" t="s">
-        <v>813</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>785</v>
-      </c>
-      <c r="R18" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="19">
@@ -6164,52 +6146,52 @@
         <v>321</v>
       </c>
       <c r="C19" t="s">
+        <v>813</v>
+      </c>
+      <c r="D19" t="s">
+        <v>814</v>
+      </c>
+      <c r="E19" t="s">
         <v>815</v>
       </c>
-      <c r="D19" t="s">
+      <c r="F19" t="s">
         <v>816</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>817</v>
       </c>
-      <c r="F19" t="s">
+      <c r="H19" t="s">
         <v>818</v>
       </c>
-      <c r="G19" t="s">
+      <c r="I19" t="s">
         <v>819</v>
       </c>
-      <c r="H19" t="s">
+      <c r="J19" t="s">
         <v>820</v>
       </c>
-      <c r="I19" t="s">
+      <c r="K19" t="s">
         <v>821</v>
       </c>
-      <c r="J19" t="s">
+      <c r="L19" t="s">
         <v>822</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>823</v>
       </c>
-      <c r="L19" t="s">
+      <c r="N19" t="s">
         <v>824</v>
       </c>
-      <c r="M19" t="s">
+      <c r="O19" t="s">
         <v>825</v>
       </c>
-      <c r="N19" t="s">
+      <c r="P19" t="s">
         <v>826</v>
       </c>
-      <c r="O19" t="s">
+      <c r="Q19" t="s">
         <v>827</v>
       </c>
-      <c r="P19" t="s">
-        <v>828</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>829</v>
-      </c>
       <c r="R19" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="20">
@@ -6220,52 +6202,52 @@
         <v>339</v>
       </c>
       <c r="C20" t="s">
+        <v>828</v>
+      </c>
+      <c r="D20" t="s">
+        <v>829</v>
+      </c>
+      <c r="E20" t="s">
         <v>830</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>831</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" t="s">
         <v>832</v>
       </c>
-      <c r="F20" t="s">
+      <c r="H20" t="s">
         <v>833</v>
       </c>
-      <c r="G20" t="s">
+      <c r="I20" t="s">
         <v>834</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>835</v>
       </c>
-      <c r="I20" t="s">
+      <c r="K20" t="s">
         <v>836</v>
       </c>
-      <c r="J20" t="s">
+      <c r="L20" t="s">
         <v>837</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>838</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>839</v>
       </c>
-      <c r="M20" t="s">
+      <c r="O20" t="s">
         <v>840</v>
       </c>
-      <c r="N20" t="s">
+      <c r="P20" t="s">
         <v>841</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>842</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>843</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>844</v>
-      </c>
-      <c r="R20" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="21">
@@ -6276,52 +6258,52 @@
         <v>357</v>
       </c>
       <c r="C21" t="s">
+        <v>844</v>
+      </c>
+      <c r="D21" t="s">
+        <v>845</v>
+      </c>
+      <c r="E21" t="s">
         <v>846</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F21" t="s">
         <v>847</v>
       </c>
-      <c r="E21" t="s">
+      <c r="G21" t="s">
         <v>848</v>
       </c>
-      <c r="F21" t="s">
+      <c r="H21" t="s">
         <v>849</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I21" t="s">
         <v>850</v>
       </c>
-      <c r="H21" t="s">
+      <c r="J21" t="s">
         <v>851</v>
       </c>
-      <c r="I21" t="s">
+      <c r="K21" t="s">
         <v>852</v>
       </c>
-      <c r="J21" t="s">
+      <c r="L21" t="s">
         <v>853</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>854</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>855</v>
       </c>
-      <c r="M21" t="s">
+      <c r="O21" t="s">
         <v>856</v>
       </c>
-      <c r="N21" t="s">
+      <c r="P21" t="s">
         <v>857</v>
-      </c>
-      <c r="O21" t="s">
-        <v>858</v>
-      </c>
-      <c r="P21" t="s">
-        <v>859</v>
       </c>
       <c r="Q21" t="s">
         <v>142</v>
       </c>
       <c r="R21" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="22">
@@ -6332,52 +6314,52 @@
         <v>375</v>
       </c>
       <c r="C22" t="s">
+        <v>859</v>
+      </c>
+      <c r="D22" t="s">
+        <v>860</v>
+      </c>
+      <c r="E22" t="s">
         <v>861</v>
       </c>
-      <c r="D22" t="s">
+      <c r="F22" t="s">
         <v>862</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>863</v>
       </c>
-      <c r="F22" t="s">
+      <c r="H22" t="s">
         <v>864</v>
       </c>
-      <c r="G22" t="s">
+      <c r="I22" t="s">
         <v>865</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
         <v>866</v>
       </c>
-      <c r="I22" t="s">
+      <c r="K22" t="s">
         <v>867</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>868</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>869</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>870</v>
       </c>
-      <c r="M22" t="s">
+      <c r="O22" t="s">
         <v>871</v>
       </c>
-      <c r="N22" t="s">
+      <c r="P22" t="s">
         <v>872</v>
       </c>
-      <c r="O22" t="s">
+      <c r="Q22" t="s">
         <v>873</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>874</v>
-      </c>
-      <c r="Q22" t="s">
-        <v>875</v>
-      </c>
-      <c r="R22" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="23">
@@ -6388,52 +6370,52 @@
         <v>393</v>
       </c>
       <c r="C23" t="s">
+        <v>875</v>
+      </c>
+      <c r="D23" t="s">
+        <v>876</v>
+      </c>
+      <c r="E23" t="s">
         <v>877</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>878</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" t="s">
         <v>879</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>880</v>
       </c>
-      <c r="G23" t="s">
+      <c r="I23" t="s">
         <v>881</v>
       </c>
-      <c r="H23" t="s">
+      <c r="J23" t="s">
         <v>882</v>
       </c>
-      <c r="I23" t="s">
+      <c r="K23" t="s">
         <v>883</v>
       </c>
-      <c r="J23" t="s">
+      <c r="L23" t="s">
         <v>884</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>885</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>886</v>
       </c>
-      <c r="M23" t="s">
+      <c r="O23" t="s">
         <v>887</v>
       </c>
-      <c r="N23" t="s">
+      <c r="P23" t="s">
         <v>888</v>
       </c>
-      <c r="O23" t="s">
+      <c r="Q23" t="s">
         <v>889</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>890</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>891</v>
-      </c>
-      <c r="R23" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="24">
@@ -6444,52 +6426,52 @@
         <v>410</v>
       </c>
       <c r="C24" t="s">
+        <v>891</v>
+      </c>
+      <c r="D24" t="s">
+        <v>892</v>
+      </c>
+      <c r="E24" t="s">
         <v>893</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>894</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>895</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>896</v>
       </c>
-      <c r="G24" t="s">
+      <c r="I24" t="s">
         <v>897</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
         <v>898</v>
       </c>
-      <c r="I24" t="s">
+      <c r="K24" t="s">
         <v>899</v>
       </c>
-      <c r="J24" t="s">
+      <c r="L24" t="s">
         <v>900</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>901</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>902</v>
       </c>
-      <c r="M24" t="s">
+      <c r="O24" t="s">
         <v>903</v>
       </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
         <v>904</v>
       </c>
-      <c r="O24" t="s">
+      <c r="Q24" t="s">
         <v>905</v>
       </c>
-      <c r="P24" t="s">
-        <v>906</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>907</v>
-      </c>
       <c r="R24" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="25">
@@ -6500,52 +6482,52 @@
         <v>428</v>
       </c>
       <c r="C25" t="s">
+        <v>906</v>
+      </c>
+      <c r="D25" t="s">
+        <v>907</v>
+      </c>
+      <c r="E25" t="s">
         <v>908</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>909</v>
       </c>
-      <c r="E25" t="s">
+      <c r="G25" t="s">
         <v>910</v>
       </c>
-      <c r="F25" t="s">
+      <c r="H25" t="s">
         <v>911</v>
       </c>
-      <c r="G25" t="s">
+      <c r="I25" t="s">
         <v>912</v>
       </c>
-      <c r="H25" t="s">
+      <c r="J25" t="s">
         <v>913</v>
       </c>
-      <c r="I25" t="s">
+      <c r="K25" t="s">
         <v>914</v>
       </c>
-      <c r="J25" t="s">
+      <c r="L25" t="s">
         <v>915</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>916</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>917</v>
       </c>
-      <c r="M25" t="s">
+      <c r="O25" t="s">
         <v>918</v>
       </c>
-      <c r="N25" t="s">
+      <c r="P25" t="s">
         <v>919</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>920</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>921</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>922</v>
-      </c>
-      <c r="R25" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="26">
@@ -6556,332 +6538,332 @@
         <v>446</v>
       </c>
       <c r="C26" t="s">
+        <v>922</v>
+      </c>
+      <c r="D26" t="s">
+        <v>923</v>
+      </c>
+      <c r="E26" t="s">
         <v>924</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>925</v>
       </c>
-      <c r="E26" t="s">
+      <c r="G26" t="s">
         <v>926</v>
       </c>
-      <c r="F26" t="s">
+      <c r="H26" t="s">
         <v>927</v>
       </c>
-      <c r="G26" t="s">
+      <c r="I26" t="s">
         <v>928</v>
       </c>
-      <c r="H26" t="s">
+      <c r="J26" t="s">
         <v>929</v>
       </c>
-      <c r="I26" t="s">
+      <c r="K26" t="s">
         <v>930</v>
       </c>
-      <c r="J26" t="s">
+      <c r="L26" t="s">
         <v>931</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>932</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>933</v>
       </c>
-      <c r="M26" t="s">
+      <c r="O26" t="s">
         <v>934</v>
       </c>
-      <c r="N26" t="s">
+      <c r="P26" t="s">
         <v>935</v>
       </c>
-      <c r="O26" t="s">
+      <c r="Q26" t="s">
         <v>936</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>937</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>938</v>
-      </c>
-      <c r="R26" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
+        <v>462</v>
+      </c>
+      <c r="B27" t="s">
         <v>463</v>
       </c>
-      <c r="B27" t="s">
-        <v>464</v>
-      </c>
       <c r="C27" t="s">
+        <v>938</v>
+      </c>
+      <c r="D27" t="s">
+        <v>939</v>
+      </c>
+      <c r="E27" t="s">
         <v>940</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>941</v>
       </c>
-      <c r="E27" t="s">
+      <c r="G27" t="s">
         <v>942</v>
       </c>
-      <c r="F27" t="s">
+      <c r="H27" t="s">
         <v>943</v>
       </c>
-      <c r="G27" t="s">
+      <c r="I27" t="s">
         <v>944</v>
       </c>
-      <c r="H27" t="s">
+      <c r="J27" t="s">
         <v>945</v>
       </c>
-      <c r="I27" t="s">
+      <c r="K27" t="s">
         <v>946</v>
       </c>
-      <c r="J27" t="s">
+      <c r="L27" t="s">
         <v>947</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>948</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>949</v>
       </c>
-      <c r="M27" t="s">
+      <c r="O27" t="s">
         <v>950</v>
       </c>
-      <c r="N27" t="s">
+      <c r="P27" t="s">
         <v>951</v>
       </c>
-      <c r="O27" t="s">
+      <c r="Q27" t="s">
         <v>952</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>953</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>954</v>
-      </c>
-      <c r="R27" t="s">
-        <v>955</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
+        <v>480</v>
+      </c>
+      <c r="B28" t="s">
         <v>481</v>
       </c>
-      <c r="B28" t="s">
-        <v>482</v>
-      </c>
       <c r="C28" t="s">
+        <v>954</v>
+      </c>
+      <c r="D28" t="s">
+        <v>955</v>
+      </c>
+      <c r="E28" t="s">
         <v>956</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>957</v>
       </c>
-      <c r="E28" t="s">
+      <c r="G28" t="s">
         <v>958</v>
       </c>
-      <c r="F28" t="s">
+      <c r="H28" t="s">
         <v>959</v>
       </c>
-      <c r="G28" t="s">
+      <c r="I28" t="s">
         <v>960</v>
       </c>
-      <c r="H28" t="s">
+      <c r="J28" t="s">
         <v>961</v>
       </c>
-      <c r="I28" t="s">
+      <c r="K28" t="s">
         <v>962</v>
       </c>
-      <c r="J28" t="s">
+      <c r="L28" t="s">
         <v>963</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>964</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>965</v>
       </c>
-      <c r="M28" t="s">
+      <c r="O28" t="s">
         <v>966</v>
       </c>
-      <c r="N28" t="s">
+      <c r="P28" t="s">
         <v>967</v>
       </c>
-      <c r="O28" t="s">
-        <v>968</v>
-      </c>
-      <c r="P28" t="s">
-        <v>969</v>
-      </c>
       <c r="Q28" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="R28" t="s">
-        <v>970</v>
+        <v>936</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="B29" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C29" t="s">
+        <v>968</v>
+      </c>
+      <c r="D29" t="s">
+        <v>969</v>
+      </c>
+      <c r="E29" t="s">
+        <v>970</v>
+      </c>
+      <c r="F29" t="s">
         <v>971</v>
       </c>
-      <c r="D29" t="s">
+      <c r="G29" t="s">
         <v>972</v>
       </c>
-      <c r="E29" t="s">
+      <c r="H29" t="s">
         <v>973</v>
       </c>
-      <c r="F29" t="s">
+      <c r="I29" t="s">
         <v>974</v>
       </c>
-      <c r="G29" t="s">
+      <c r="J29" t="s">
         <v>975</v>
       </c>
-      <c r="H29" t="s">
+      <c r="K29" t="s">
         <v>976</v>
       </c>
-      <c r="I29" t="s">
+      <c r="L29" t="s">
         <v>977</v>
       </c>
-      <c r="J29" t="s">
+      <c r="M29" t="s">
         <v>978</v>
       </c>
-      <c r="K29" t="s">
+      <c r="N29" t="s">
         <v>979</v>
       </c>
-      <c r="L29" t="s">
+      <c r="O29" t="s">
         <v>980</v>
       </c>
-      <c r="M29" t="s">
+      <c r="P29" t="s">
         <v>981</v>
       </c>
-      <c r="N29" t="s">
+      <c r="Q29" t="s">
         <v>982</v>
       </c>
-      <c r="O29" t="s">
+      <c r="R29" t="s">
         <v>983</v>
-      </c>
-      <c r="P29" t="s">
-        <v>984</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>985</v>
-      </c>
-      <c r="R29" t="s">
-        <v>986</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B30" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C30" t="s">
+        <v>713</v>
+      </c>
+      <c r="D30" t="s">
+        <v>984</v>
+      </c>
+      <c r="E30" t="s">
+        <v>985</v>
+      </c>
+      <c r="F30" t="s">
+        <v>986</v>
+      </c>
+      <c r="G30" t="s">
         <v>987</v>
       </c>
-      <c r="D30" t="s">
+      <c r="H30" t="s">
+        <v>986</v>
+      </c>
+      <c r="I30" t="s">
         <v>988</v>
       </c>
-      <c r="E30" t="s">
+      <c r="J30" t="s">
         <v>989</v>
       </c>
-      <c r="F30" t="s">
+      <c r="K30" t="s">
         <v>990</v>
       </c>
-      <c r="G30" t="s">
+      <c r="L30" t="s">
         <v>991</v>
       </c>
-      <c r="H30" t="s">
+      <c r="M30" t="s">
         <v>992</v>
       </c>
-      <c r="I30" t="s">
+      <c r="N30" t="s">
         <v>993</v>
       </c>
-      <c r="J30" t="s">
+      <c r="O30" t="s">
+        <v>459</v>
+      </c>
+      <c r="P30" t="s">
         <v>994</v>
       </c>
-      <c r="K30" t="s">
+      <c r="Q30" t="s">
         <v>995</v>
       </c>
-      <c r="L30" t="s">
-        <v>996</v>
-      </c>
-      <c r="M30" t="s">
-        <v>997</v>
-      </c>
-      <c r="N30" t="s">
-        <v>998</v>
-      </c>
-      <c r="O30" t="s">
-        <v>999</v>
-      </c>
-      <c r="P30" t="s">
-        <v>1000</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>1001</v>
-      </c>
       <c r="R30" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B31" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C31" t="s">
+        <v>996</v>
+      </c>
+      <c r="D31" t="s">
+        <v>997</v>
+      </c>
+      <c r="E31" t="s">
+        <v>998</v>
+      </c>
+      <c r="F31" t="s">
+        <v>999</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1000</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1001</v>
+      </c>
+      <c r="I31" t="s">
         <v>1002</v>
       </c>
-      <c r="D31" t="s">
+      <c r="J31" t="s">
         <v>1003</v>
       </c>
-      <c r="E31" t="s">
+      <c r="K31" t="s">
         <v>1004</v>
       </c>
-      <c r="F31" t="s">
+      <c r="L31" t="s">
         <v>1005</v>
       </c>
-      <c r="G31" t="s">
+      <c r="M31" t="s">
         <v>1006</v>
       </c>
-      <c r="H31" t="s">
+      <c r="N31" t="s">
         <v>1007</v>
       </c>
-      <c r="I31" t="s">
+      <c r="O31" t="s">
         <v>1008</v>
       </c>
-      <c r="J31" t="s">
+      <c r="P31" t="s">
         <v>1009</v>
       </c>
-      <c r="K31" t="s">
+      <c r="Q31" t="s">
         <v>1010</v>
       </c>
-      <c r="L31" t="s">
+      <c r="R31" t="s">
         <v>1011</v>
-      </c>
-      <c r="M31" t="s">
-        <v>1012</v>
-      </c>
-      <c r="N31" t="s">
-        <v>1013</v>
-      </c>
-      <c r="O31" t="s">
-        <v>1014</v>
-      </c>
-      <c r="P31" t="s">
-        <v>1015</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>1016</v>
-      </c>
-      <c r="R31" t="s">
-        <v>1017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>